<commit_message>
codigo de graficos teste adicionado
</commit_message>
<xml_diff>
--- a/teste/dados_rto.xlsx
+++ b/teste/dados_rto.xlsx
@@ -484,7 +484,7 @@
         <v>1.2</v>
       </c>
       <c r="E2">
-        <v>10.17</v>
+        <v>10</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -493,7 +493,7 @@
         <v>0.08</v>
       </c>
       <c r="H2">
-        <v>0.2198188426595857</v>
+        <v>0.135187728937729</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -507,19 +507,19 @@
         <v>0.25</v>
       </c>
       <c r="D3">
-        <v>1.245200187560044</v>
+        <v>1.230061164574647</v>
       </c>
       <c r="E3">
-        <v>9.706424110744331</v>
+        <v>9.694302871522011</v>
       </c>
       <c r="F3">
-        <v>0.01375843780634723</v>
+        <v>0.01956501320124453</v>
       </c>
       <c r="G3">
-        <v>2.006253431714941</v>
+        <v>2.584752575149968</v>
       </c>
       <c r="H3">
-        <v>0.3715425636901243</v>
+        <v>0.2551642340404257</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -533,19 +533,19 @@
         <v>0.25</v>
       </c>
       <c r="D4">
-        <v>1.292122023736629</v>
+        <v>1.261271353644799</v>
       </c>
       <c r="E4">
-        <v>9.224703689993946</v>
+        <v>9.375937720795555</v>
       </c>
       <c r="F4">
-        <v>0.02782518005923739</v>
+        <v>0.03903804594228661</v>
       </c>
       <c r="G4">
-        <v>1.853811439729191</v>
+        <v>2.5332113183011</v>
       </c>
       <c r="H4">
-        <v>0.3697108960406665</v>
+        <v>0.2534275749034835</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -559,19 +559,19 @@
         <v>0.25</v>
       </c>
       <c r="D5">
-        <v>1.340541602450056</v>
+        <v>1.29304035520393</v>
       </c>
       <c r="E5">
-        <v>8.7286938783721</v>
+        <v>9.052117772373517</v>
       </c>
       <c r="F5">
-        <v>0.0429189358098474</v>
+        <v>0.05916742341105483</v>
       </c>
       <c r="G5">
-        <v>1.705824462615348</v>
+        <v>2.482476542261214</v>
       </c>
       <c r="H5">
-        <v>0.3676028656954948</v>
+        <v>0.2516493274891522</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -585,19 +585,19 @@
         <v>0.25</v>
       </c>
       <c r="D6">
-        <v>1.390452569962527</v>
+        <v>1.325364868139073</v>
       </c>
       <c r="E6">
-        <v>8.218632150982568</v>
+        <v>8.722883968236125</v>
       </c>
       <c r="F6">
-        <v>0.05913748596344727</v>
+        <v>0.07996789390766709</v>
       </c>
       <c r="G6">
-        <v>1.563936426018927</v>
+        <v>2.432632432584629</v>
       </c>
       <c r="H6">
-        <v>0.3651733203701772</v>
+        <v>0.2498275236607224</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -611,19 +611,19 @@
         <v>0.25</v>
       </c>
       <c r="D7">
-        <v>1.441835698986062</v>
+        <v>1.358240460986729</v>
       </c>
       <c r="E7">
-        <v>7.694889140712592</v>
+        <v>8.388286721796272</v>
       </c>
       <c r="F7">
-        <v>0.07658033845740704</v>
+        <v>0.1014531045424298</v>
       </c>
       <c r="G7">
-        <v>1.429822163071999</v>
+        <v>2.383766355068916</v>
       </c>
       <c r="H7">
-        <v>0.3623731184815424</v>
+        <v>0.2479596456207434</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -637,19 +637,19 @@
         <v>0.25</v>
       </c>
       <c r="D8">
-        <v>1.494656585914394</v>
+        <v>1.391661414455903</v>
       </c>
       <c r="E8">
-        <v>7.157978861668961</v>
+        <v>8.048386963831456</v>
       </c>
       <c r="F8">
-        <v>0.09534298501736831</v>
+        <v>0.123635280967621</v>
       </c>
       <c r="G8">
-        <v>1.305082951324532</v>
+        <v>2.335970363374372</v>
       </c>
       <c r="H8">
-        <v>0.3591501286156472</v>
+        <v>0.2460424919860801</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -663,19 +663,19 @@
         <v>0.25</v>
       </c>
       <c r="D9">
-        <v>1.548863261367992</v>
+        <v>1.425620526173195</v>
       </c>
       <c r="E9">
-        <v>6.608564559549235</v>
+        <v>7.703257452797909</v>
       </c>
       <c r="F9">
-        <v>0.1155088818367327</v>
+        <v>0.1465248406067019</v>
       </c>
       <c r="G9">
-        <v>1.191130982183369</v>
+        <v>2.289342796332378</v>
       </c>
       <c r="H9">
-        <v>0.3554495917670101</v>
+        <v>0.2440719974017905</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -689,19 +689,19 @@
         <v>0.25</v>
       </c>
       <c r="D10">
-        <v>1.604383490611314</v>
+        <v>1.460108866567499</v>
       </c>
       <c r="E10">
-        <v>6.047462127930769</v>
+        <v>7.352984430853897</v>
       </c>
       <c r="F10">
-        <v>0.1371390170398632</v>
+        <v>0.1701299214689206</v>
       </c>
       <c r="G10">
-        <v>1.089106073140937</v>
+        <v>2.243990473217152</v>
       </c>
       <c r="H10">
-        <v>0.3512124910109985</v>
+        <v>0.2420430026749867</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -715,19 +715,19 @@
         <v>0.25</v>
       </c>
       <c r="D11">
-        <v>1.661121334984533</v>
+        <v>1.495115471349499</v>
       </c>
       <c r="E11">
-        <v>5.475645146559579</v>
+        <v>6.997669732924798</v>
       </c>
       <c r="F11">
-        <v>0.1602589353919247</v>
+        <v>0.194455804033384</v>
       </c>
       <c r="G11">
-        <v>0.9998697714902988</v>
+        <v>2.200031691161895</v>
       </c>
       <c r="H11">
-        <v>0.3463699209112795</v>
+        <v>0.239948958172568</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -741,19 +741,19 @@
         <v>0.25</v>
       </c>
       <c r="D12">
-        <v>1.718951847510803</v>
+        <v>1.530626952630354</v>
       </c>
       <c r="E12">
-        <v>4.894261975673999</v>
+        <v>6.637433480315335</v>
       </c>
       <c r="F12">
-        <v>0.1848428670795613</v>
+        <v>0.2195041971387745</v>
       </c>
       <c r="G12">
-        <v>0.9241209127313187</v>
+        <v>2.157600324278091</v>
       </c>
       <c r="H12">
-        <v>0.3408307605171383</v>
+        <v>0.2377815360115555</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -767,19 +767,19 @@
         <v>0.25</v>
       </c>
       <c r="D13">
-        <v>1.777711994697241</v>
+        <v>1.566626994617957</v>
       </c>
       <c r="E13">
-        <v>4.30468027798168</v>
+        <v>6.272417620394417</v>
       </c>
       <c r="F13">
-        <v>0.2107933076085911</v>
+        <v>0.2452723450152412</v>
       </c>
       <c r="G13">
-        <v>0.8626813456203928</v>
+        <v>2.116851510233683</v>
       </c>
       <c r="H13">
-        <v>0.3344584433952746</v>
+        <v>0.2355301172473205</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -793,19 +793,19 @@
         <v>0.25</v>
       </c>
       <c r="D14">
-        <v>1.837184529728484</v>
+        <v>1.603095706443778</v>
       </c>
       <c r="E14">
-        <v>3.708584064549552</v>
+        <v>5.902790506512941</v>
       </c>
       <c r="F14">
-        <v>0.2379126747591827</v>
+        <v>0.2717519023736472</v>
       </c>
       <c r="G14">
-        <v>0.8170548388118836</v>
+        <v>2.077969535632409</v>
       </c>
       <c r="H14">
-        <v>0.3270283644021128</v>
+        <v>0.2331811006068292</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -819,19 +819,19 @@
         <v>0.25</v>
       </c>
       <c r="D15">
-        <v>1.897067501796379</v>
+        <v>1.640008773411502</v>
       </c>
       <c r="E15">
-        <v>3.108178608843957</v>
+        <v>5.52875296928673</v>
       </c>
       <c r="F15">
-        <v>0.2658592426582192</v>
+        <v>0.298927501710494</v>
       </c>
       <c r="G15">
-        <v>0.7905704258025728</v>
+        <v>2.041179032281789</v>
       </c>
       <c r="H15">
-        <v>0.3181457095584918</v>
+        <v>0.2307169582559074</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -845,19 +845,19 @@
         <v>0.25</v>
       </c>
       <c r="D16">
-        <v>1.956915305225231</v>
+        <v>1.67733632997442</v>
       </c>
       <c r="E16">
-        <v>2.506615797900139</v>
+        <v>5.150546462828657</v>
       </c>
       <c r="F16">
-        <v>0.2940747685556034</v>
+        <v>0.3267749048084885</v>
       </c>
       <c r="G16">
-        <v>0.7911289628781146</v>
+        <v>2.006761106614411</v>
       </c>
       <c r="H16">
-        <v>0.3070693166735627</v>
+        <v>0.2281149212617001</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -871,19 +871,19 @@
         <v>0.25</v>
       </c>
       <c r="D17">
-        <v>2.016012463649007</v>
+        <v>1.715041438192036</v>
       </c>
       <c r="E17">
-        <v>1.908976348000787</v>
+        <v>4.768464181499732</v>
       </c>
       <c r="F17">
-        <v>0.321660961450897</v>
+        <v>0.3552585827199661</v>
       </c>
       <c r="G17">
-        <v>0.8392943510167811</v>
+        <v>1.97507709552527</v>
       </c>
       <c r="H17">
-        <v>0.2922767439605348</v>
+        <v>0.2253451140547482</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -897,19 +897,19 @@
         <v>0.25</v>
       </c>
       <c r="D18">
-        <v>2.07306669933687</v>
+        <v>1.753078162924562</v>
       </c>
       <c r="E18">
-        <v>1.324910750156073</v>
+        <v>4.382865219067759</v>
       </c>
       <c r="F18">
-        <v>0.3471889822339113</v>
+        <v>0.384328687529078</v>
       </c>
       <c r="G18">
-        <v>0.9979895799488291</v>
+        <v>1.94660423441623</v>
       </c>
       <c r="H18">
-        <v>0.2701893769640245</v>
+        <v>0.2223678356001359</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -923,19 +923,19 @@
         <v>0.25</v>
       </c>
       <c r="D19">
-        <v>2.125332571467569</v>
+        <v>1.791388330520623</v>
       </c>
       <c r="E19">
-        <v>0.7772621566703322</v>
+        <v>3.994198911143533</v>
       </c>
       <c r="F19">
-        <v>0.368624517011227</v>
+        <v>0.4139163663733543</v>
       </c>
       <c r="G19">
-        <v>1.498514638433982</v>
+        <v>1.921991681833087</v>
       </c>
       <c r="H19">
-        <v>0.2310527199541394</v>
+        <v>0.2191295619388361</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -949,19 +949,19 @@
         <v>0.25</v>
       </c>
       <c r="D20">
-        <v>2.166361559643355</v>
+        <v>1.829897789896376</v>
       </c>
       <c r="E20">
-        <v>0.3276453769657671</v>
+        <v>3.6030330991757</v>
       </c>
       <c r="F20">
-        <v>0.3846157797549108</v>
+        <v>0.4439283224449158</v>
       </c>
       <c r="G20">
-        <v>3.035139585869074</v>
+        <v>1.902149549946629</v>
       </c>
       <c r="H20">
-        <v>0.153768940019126</v>
+        <v>0.2155567795842495</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -975,19 +975,19 @@
         <v>0.25</v>
       </c>
       <c r="D21">
-        <v>2.186730075514632</v>
+        <v>1.868510257712079</v>
       </c>
       <c r="E21">
-        <v>0.07520570070900059</v>
+        <v>3.210101528749905</v>
       </c>
       <c r="F21">
-        <v>0.3970285334033221</v>
+        <v>0.4742385246842796</v>
       </c>
       <c r="G21">
-        <v>5.665403643454165</v>
+        <v>1.888397849171365</v>
       </c>
       <c r="H21">
-        <v>0.05136162872851624</v>
+        <v>0.2115463185397637</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1001,19 +1001,19 @@
         <v>0.25</v>
       </c>
       <c r="D22">
-        <v>2.189080385832337</v>
+        <v>1.907098447098341</v>
       </c>
       <c r="E22">
-        <v>0.0001636660491364881</v>
+        <v>2.816373493230398</v>
       </c>
       <c r="F22">
-        <v>0.4084018919677562</v>
+        <v>0.5046769974083647</v>
       </c>
       <c r="G22">
-        <v>7.204704379199374</v>
+        <v>1.882726517769569</v>
       </c>
       <c r="H22">
-        <v>0.0001289394587689012</v>
+        <v>0.2069495771220418</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1027,19 +1027,19 @@
         <v>0.25</v>
       </c>
       <c r="D23">
-        <v>2.18683640710826</v>
+        <v>1.945490031811677</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>2.423166519672241</v>
       </c>
       <c r="F23">
-        <v>0.4196221928503182</v>
+        <v>0.5350135572579119</v>
       </c>
       <c r="G23">
-        <v>7.281291603077083</v>
+        <v>1.88827220519703</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>0.201545713662244</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1053,19 +1053,19 @@
         <v>0.25</v>
       </c>
       <c r="D24">
-        <v>2.184594647769722</v>
+        <v>1.983445205230405</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>2.032331883026431</v>
       </c>
       <c r="F24">
-        <v>0.4308309895430043</v>
+        <v>0.5649349183065128</v>
       </c>
       <c r="G24">
-        <v>7.281518694130812</v>
+        <v>1.910248887877363</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>0.1949938523523468</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1079,19 +1079,19 @@
         <v>0.25</v>
       </c>
       <c r="D25">
-        <v>2.18235518644261</v>
+        <v>2.020618490887375</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>1.646581796337372</v>
       </c>
       <c r="F25">
-        <v>0.4420282961785635</v>
+        <v>0.5940123526389429</v>
       </c>
       <c r="G25">
-        <v>7.281742655160879</v>
+        <v>1.957895537623406</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>0.1867429667006245</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1105,19 +1105,19 @@
         <v>0.25</v>
       </c>
       <c r="D26">
-        <v>2.180118020820623</v>
+        <v>2.056490314094515</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>1.27010313744045</v>
       </c>
       <c r="F26">
-        <v>0.4532141242885017</v>
+        <v>0.6216594863273229</v>
       </c>
       <c r="G26">
-        <v>7.281966394588381</v>
+        <v>2.04888666398219</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>0.1758507601097975</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1131,19 +1131,19 @@
         <v>0.25</v>
       </c>
       <c r="D27">
-        <v>2.177883148550396</v>
+        <v>2.09023587758007</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>0.9098022976070663</v>
       </c>
       <c r="F27">
-        <v>0.4643884856396339</v>
+        <v>0.6470906591349083</v>
       </c>
       <c r="G27">
-        <v>7.282189904133226</v>
+        <v>2.220102745366708</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>0.160597435529722</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1157,19 +1157,19 @@
         <v>0.25</v>
       </c>
       <c r="D28">
-        <v>2.175650567280981</v>
+        <v>2.120461326266817</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>0.5779901434284483</v>
       </c>
       <c r="F28">
-        <v>0.4755513919867109</v>
+        <v>0.6693393600437654</v>
       </c>
       <c r="G28">
-        <v>7.282413184590514</v>
+        <v>2.554345829326926</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>0.1376769085044747</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1183,19 +1183,19 @@
         <v>0.25</v>
       </c>
       <c r="D29">
-        <v>2.173420274663837</v>
+        <v>2.144721277660468</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>0.2977438888478305</v>
       </c>
       <c r="F29">
-        <v>0.4867028550724317</v>
+        <v>0.687545740695289</v>
       </c>
       <c r="G29">
-        <v>7.282636236157221</v>
+        <v>3.225632555992342</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <v>0.1014013351610669</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1209,19 +1209,19 @@
         <v>0.25</v>
       </c>
       <c r="D30">
-        <v>2.171192268352831</v>
+        <v>2.159447753005895</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>0.1051900611120846</v>
       </c>
       <c r="F30">
-        <v>0.4978428866274563</v>
+        <v>0.7018186336261312</v>
       </c>
       <c r="G30">
-        <v>7.282859059070623</v>
+        <v>4.371730066026622</v>
       </c>
       <c r="H30">
-        <v>0</v>
+        <v>0.05074989722327612</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1235,19 +1235,19 @@
         <v>0.25</v>
       </c>
       <c r="D31">
-        <v>2.168966546004238</v>
+        <v>2.163427348291259</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>0.01559760035816608</v>
       </c>
       <c r="F31">
-        <v>0.5089714983704179</v>
+        <v>0.7137258040690134</v>
       </c>
       <c r="G31">
-        <v>7.283081653564933</v>
+        <v>5.466704780864711</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>0.009270349049419186</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1261,16 +1261,16 @@
         <v>0.25</v>
       </c>
       <c r="D32">
-        <v>2.166743105277615</v>
+        <v>2.161595788090185</v>
       </c>
       <c r="E32">
         <v>0</v>
       </c>
       <c r="F32">
-        <v>0.5200887020035319</v>
+        <v>0.7248582127401449</v>
       </c>
       <c r="G32">
-        <v>7.283304019874225</v>
+        <v>5.783703093506416</v>
       </c>
       <c r="H32">
         <v>0</v>
@@ -1287,16 +1287,16 @@
         <v>0.25</v>
       </c>
       <c r="D33">
-        <v>2.16452194383457</v>
+        <v>2.159379903309231</v>
       </c>
       <c r="E33">
         <v>0</v>
       </c>
       <c r="F33">
-        <v>0.5311945092187551</v>
+        <v>0.7359376366449147</v>
       </c>
       <c r="G33">
-        <v>7.283526158232367</v>
+        <v>5.78404046885179</v>
       </c>
       <c r="H33">
         <v>0</v>
@@ -1313,16 +1313,16 @@
         <v>0.25</v>
       </c>
       <c r="D34">
-        <v>2.162303059338563</v>
+        <v>2.157166290003559</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="F34">
-        <v>0.5422889316987924</v>
+        <v>0.7470057031732772</v>
       </c>
       <c r="G34">
-        <v>7.28374806887303</v>
+        <v>5.784261793519669</v>
       </c>
       <c r="H34">
         <v>0</v>
@@ -1339,16 +1339,16 @@
         <v>0.25</v>
       </c>
       <c r="D35">
-        <v>2.160086449455447</v>
+        <v>2.154954945907048</v>
       </c>
       <c r="E35">
         <v>0</v>
       </c>
       <c r="F35">
-        <v>0.553371981114371</v>
+        <v>0.7580624236558285</v>
       </c>
       <c r="G35">
-        <v>7.283969752029658</v>
+        <v>5.784482953945356</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -1365,16 +1365,16 @@
         <v>0.25</v>
       </c>
       <c r="D36">
-        <v>2.157872111853471</v>
+        <v>2.152745868693491</v>
       </c>
       <c r="E36">
         <v>0</v>
       </c>
       <c r="F36">
-        <v>0.5644436691242525</v>
+        <v>0.7691078097236117</v>
       </c>
       <c r="G36">
-        <v>7.284191207935446</v>
+        <v>5.784703883503315</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -1391,16 +1391,16 @@
         <v>0.25</v>
       </c>
       <c r="D37">
-        <v>2.155660044203273</v>
+        <v>2.150539056039065</v>
       </c>
       <c r="E37">
         <v>0</v>
       </c>
       <c r="F37">
-        <v>0.575504007375245</v>
+        <v>0.7801418729957449</v>
       </c>
       <c r="G37">
-        <v>7.284412436823356</v>
+        <v>5.784924586855793</v>
       </c>
       <c r="H37">
         <v>0</v>
@@ -1417,16 +1417,16 @@
         <v>0.25</v>
       </c>
       <c r="D38">
-        <v>2.153450244177879</v>
+        <v>2.148334505622327</v>
       </c>
       <c r="E38">
         <v>0</v>
       </c>
       <c r="F38">
-        <v>0.5865530075022161</v>
+        <v>0.7911646250794344</v>
       </c>
       <c r="G38">
-        <v>7.284633438926105</v>
+        <v>5.785145063944097</v>
       </c>
       <c r="H38">
         <v>0</v>
@@ -1443,16 +1443,16 @@
         <v>0.25</v>
       </c>
       <c r="D39">
-        <v>2.1512427094527</v>
+        <v>2.146132215124217</v>
       </c>
       <c r="E39">
         <v>0</v>
       </c>
       <c r="F39">
-        <v>0.5975906811281047</v>
+        <v>0.8021760775699875</v>
       </c>
       <c r="G39">
-        <v>7.284854214476177</v>
+        <v>5.785365315019084</v>
       </c>
       <c r="H39">
         <v>0</v>
@@ -1469,16 +1469,16 @@
         <v>0.25</v>
       </c>
       <c r="D40">
-        <v>2.149037437705536</v>
+        <v>2.143932182228049</v>
       </c>
       <c r="E40">
         <v>0</v>
       </c>
       <c r="F40">
-        <v>0.6086170398639326</v>
+        <v>0.8131762420508234</v>
       </c>
       <c r="G40">
-        <v>7.285074763705818</v>
+        <v>5.785585340311227</v>
       </c>
       <c r="H40">
         <v>0</v>
@@ -1495,16 +1495,16 @@
         <v>0.25</v>
       </c>
       <c r="D41">
-        <v>2.146834426616558</v>
+        <v>2.141734404619517</v>
       </c>
       <c r="E41">
         <v>0</v>
       </c>
       <c r="F41">
-        <v>0.6196320953088187</v>
+        <v>0.8241651300934869</v>
       </c>
       <c r="G41">
-        <v>7.285295086847029</v>
+        <v>5.785805140052053</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -1515,25 +1515,25 @@
         <v>4.104166666666667</v>
       </c>
       <c r="B42">
-        <v>0.01396652409312703</v>
+        <v>0.01147170103680971</v>
       </c>
       <c r="C42">
-        <v>0.2514548462597018</v>
+        <v>0.2511949688580001</v>
       </c>
       <c r="D42">
-        <v>2.153645736648322</v>
+        <v>2.145334087923702</v>
       </c>
       <c r="E42">
-        <v>1.252518660513393</v>
+        <v>1.033943247733082</v>
       </c>
       <c r="F42">
-        <v>0.6487396098620378</v>
+        <v>0.8505065866523553</v>
       </c>
       <c r="G42">
-        <v>0.0267016200880029</v>
+        <v>0.2016474951784967</v>
       </c>
       <c r="H42">
-        <v>0.1118460412685493</v>
+        <v>0.08905621808614919</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1541,25 +1541,25 @@
         <v>4.208333333333333</v>
       </c>
       <c r="B43">
-        <v>0.01396652409312703</v>
+        <v>0.01147170103680971</v>
       </c>
       <c r="C43">
-        <v>0.2529096925194027</v>
+        <v>0.2523899377160009</v>
       </c>
       <c r="D43">
-        <v>2.166946361229821</v>
+        <v>2.155663759521709</v>
       </c>
       <c r="E43">
-        <v>2.478978275885301</v>
+        <v>2.032735821329882</v>
       </c>
       <c r="F43">
-        <v>0.7011180236056238</v>
+        <v>0.9007072932194852</v>
       </c>
       <c r="G43">
-        <v>0.02231922745190233</v>
+        <v>0.1655404147378546</v>
       </c>
       <c r="H43">
-        <v>0.1336565066917518</v>
+        <v>0.1111113125528041</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1567,25 +1567,25 @@
         <v>4.3125</v>
       </c>
       <c r="B44">
-        <v>0.01396652409312703</v>
+        <v>0.01147170103680971</v>
       </c>
       <c r="C44">
-        <v>0.2543645387791034</v>
+        <v>0.2535849065740021</v>
       </c>
       <c r="D44">
-        <v>2.183686110935024</v>
+        <v>2.169520142917142</v>
       </c>
       <c r="E44">
-        <v>3.673173543564589</v>
+        <v>3.001443220475506</v>
       </c>
       <c r="F44">
-        <v>0.7609354611844148</v>
+        <v>0.9596123649736499</v>
       </c>
       <c r="G44">
-        <v>0.02075685480029876</v>
+        <v>0.1530198286709244</v>
       </c>
       <c r="H44">
-        <v>0.1431124295608868</v>
+        <v>0.1215032176230276</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1593,25 +1593,25 @@
         <v>4.416666666666667</v>
       </c>
       <c r="B45">
-        <v>0.01396652409312703</v>
+        <v>0.01147170103680971</v>
       </c>
       <c r="C45">
-        <v>0.2558193850388041</v>
+        <v>0.254779875432003</v>
       </c>
       <c r="D45">
-        <v>2.202203242876189</v>
+        <v>2.185292602046957</v>
       </c>
       <c r="E45">
-        <v>4.843454139908237</v>
+        <v>3.949119044892583</v>
       </c>
       <c r="F45">
-        <v>0.8245629315911502</v>
+        <v>1.023223860413057</v>
       </c>
       <c r="G45">
-        <v>0.01986727571059387</v>
+        <v>0.1460499080484365</v>
       </c>
       <c r="H45">
-        <v>0.1480235198441965</v>
+        <v>0.1273353350671148</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1619,25 +1619,25 @@
         <v>4.520833333333333</v>
       </c>
       <c r="B46">
-        <v>0.009999997402030975</v>
+        <v>0.009999998188783122</v>
       </c>
       <c r="C46">
-        <v>0.256861051434849</v>
+        <v>0.2558215419100011</v>
       </c>
       <c r="D46">
-        <v>2.225254116461457</v>
+        <v>2.2035335172011</v>
       </c>
       <c r="E46">
-        <v>5.601589420697604</v>
+        <v>4.733275312376302</v>
       </c>
       <c r="F46">
-        <v>0.8916674548069536</v>
+        <v>1.090304437038553</v>
       </c>
       <c r="G46">
-        <v>0.01931568959650332</v>
+        <v>0.1415684733729707</v>
       </c>
       <c r="H46">
-        <v>0.1497985790657573</v>
+        <v>0.1304010488906717</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1645,25 +1645,25 @@
         <v>4.625</v>
       </c>
       <c r="B47">
-        <v>0.009999997402030975</v>
+        <v>0.009999998188783122</v>
       </c>
       <c r="C47">
-        <v>0.2579027178308939</v>
+        <v>0.2568632083879992</v>
       </c>
       <c r="D47">
-        <v>2.248921602800766</v>
+        <v>2.22255114486153</v>
       </c>
       <c r="E47">
-        <v>6.34901316089791</v>
+        <v>5.505350306560847</v>
       </c>
       <c r="F47">
-        <v>0.9602128588474849</v>
+        <v>1.159339722216303</v>
       </c>
       <c r="G47">
-        <v>0.01883855543694846</v>
+        <v>0.1379443901758264</v>
       </c>
       <c r="H47">
-        <v>0.150952149787045</v>
+        <v>0.1324840125822739</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1671,25 +1671,25 @@
         <v>4.729166666666667</v>
       </c>
       <c r="B48">
-        <v>0.009999997402030975</v>
+        <v>0.009999998188783122</v>
       </c>
       <c r="C48">
-        <v>0.2589443842269389</v>
+        <v>0.2579048748659976</v>
       </c>
       <c r="D48">
-        <v>2.273096711146118</v>
+        <v>2.242175582705977</v>
       </c>
       <c r="E48">
-        <v>7.086339497143235</v>
+        <v>6.266371246457896</v>
       </c>
       <c r="F48">
-        <v>1.029965435368412</v>
+        <v>1.229914395490082</v>
       </c>
       <c r="G48">
-        <v>0.01841208116604288</v>
+        <v>0.1348422368198753</v>
       </c>
       <c r="H48">
-        <v>0.1516715889920706</v>
+        <v>0.1339182570471253</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1697,25 +1697,25 @@
         <v>4.833333333333333</v>
       </c>
       <c r="B49">
-        <v>0.009999997402030975</v>
+        <v>0.009999998188783122</v>
       </c>
       <c r="C49">
-        <v>0.2599860506229837</v>
+        <v>0.2589465413439958</v>
       </c>
       <c r="D49">
-        <v>2.297701587835404</v>
+        <v>2.262292106900332</v>
       </c>
       <c r="E49">
-        <v>7.814031257630253</v>
+        <v>7.017058835139452</v>
       </c>
       <c r="F49">
-        <v>1.100759039872591</v>
+        <v>1.301749220499117</v>
       </c>
       <c r="G49">
-        <v>0.01802224735380649</v>
+        <v>0.1320875487599754</v>
       </c>
       <c r="H49">
-        <v>0.1520773338520987</v>
+        <v>0.1349030196982902</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1723,25 +1723,25 @@
         <v>4.9375</v>
       </c>
       <c r="B50">
-        <v>0.009999997401711199</v>
+        <v>0.009999998060907822</v>
       </c>
       <c r="C50">
-        <v>0.2610277170189954</v>
+        <v>0.2599882078086737</v>
       </c>
       <c r="D50">
-        <v>2.322678745535621</v>
+        <v>2.282819763919518</v>
       </c>
       <c r="E50">
-        <v>8.53245123450024</v>
+        <v>7.757945704776938</v>
       </c>
       <c r="F50">
-        <v>1.172471659907426</v>
+        <v>1.374648108239052</v>
       </c>
       <c r="G50">
-        <v>0.01766018797378151</v>
+        <v>0.1295785229913029</v>
       </c>
       <c r="H50">
-        <v>0.1522502603135957</v>
+        <v>0.1355644170617218</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -1749,25 +1749,25 @@
         <v>5.041666666666667</v>
       </c>
       <c r="B51">
-        <v>0.009999997401711199</v>
+        <v>0.009999998060907822</v>
       </c>
       <c r="C51">
-        <v>0.262069383415007</v>
+        <v>0.2610298742733516</v>
       </c>
       <c r="D51">
-        <v>2.347984558673025</v>
+        <v>2.303699260792663</v>
       </c>
       <c r="E51">
-        <v>9.241893771018205</v>
+        <v>8.489443571999644</v>
       </c>
       <c r="F51">
-        <v>1.245011271755256</v>
+        <v>1.448468224278636</v>
       </c>
       <c r="G51">
-        <v>0.01732001351933676</v>
+        <v>0.1272518003828241</v>
       </c>
       <c r="H51">
-        <v>0.1522466929831273</v>
+        <v>0.1359862212242035</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1775,25 +1775,25 @@
         <v>5.145833333333334</v>
       </c>
       <c r="B52">
-        <v>0.009999997401711199</v>
+        <v>0.009999998060907822</v>
       </c>
       <c r="C52">
-        <v>0.2631110498110185</v>
+        <v>0.2620715407380296</v>
       </c>
       <c r="D52">
-        <v>2.373585170759753</v>
+        <v>2.324885915757206</v>
       </c>
       <c r="E52">
-        <v>9.942604640685111</v>
+        <v>9.211882227859032</v>
       </c>
       <c r="F52">
-        <v>1.318306951715905</v>
+        <v>1.523102602879328</v>
       </c>
       <c r="G52">
-        <v>0.01699764869000067</v>
+        <v>0.1250658748510481</v>
       </c>
       <c r="H52">
-        <v>0.1521070493407661</v>
+        <v>0.1362262677861756</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -1801,25 +1801,25 @@
         <v>5.25</v>
       </c>
       <c r="B53">
-        <v>0.009999997401711199</v>
+        <v>0.009999998060907822</v>
       </c>
       <c r="C53">
-        <v>0.2641527162070301</v>
+        <v>0.2631132072027075</v>
       </c>
       <c r="D53">
-        <v>2.399453798314235</v>
+        <v>2.346345276233348</v>
       </c>
       <c r="E53">
-        <v>10.63479413975776</v>
+        <v>9.925533727198369</v>
       </c>
       <c r="F53">
-        <v>1.392303027328623</v>
+        <v>1.598469348720029</v>
       </c>
       <c r="G53">
-        <v>0.01669017488688043</v>
+        <v>0.1229924139437977</v>
       </c>
       <c r="H53">
-        <v>0.1518610669682509</v>
+        <v>0.1363257716186922</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -1827,25 +1827,25 @@
         <v>5.354166666666667</v>
       </c>
       <c r="B54">
-        <v>0.009999997401631506</v>
+        <v>0.009999998030480454</v>
       </c>
       <c r="C54">
-        <v>0.2651943826030334</v>
+        <v>0.2641548736642159</v>
       </c>
       <c r="D54">
-        <v>2.425568769269546</v>
+        <v>2.368050228892933</v>
       </c>
       <c r="E54">
-        <v>11.31864722756244</v>
+        <v>10.63062843164556</v>
       </c>
       <c r="F54">
-        <v>1.466954843766112</v>
+        <v>1.674504526696496</v>
       </c>
       <c r="G54">
-        <v>0.01639544004655905</v>
+        <v>0.121011382065703</v>
       </c>
       <c r="H54">
-        <v>0.1515310960909015</v>
+        <v>0.1363148888057276</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -1853,25 +1853,25 @@
         <v>5.458333333333334</v>
       </c>
       <c r="B55">
-        <v>0.009999997401631506</v>
+        <v>0.009999998030480454</v>
       </c>
       <c r="C55">
-        <v>0.2662360489990367</v>
+        <v>0.2651965401257242</v>
       </c>
       <c r="D55">
-        <v>2.451912698820466</v>
+        <v>2.389979080787206</v>
       </c>
       <c r="E55">
-        <v>11.99432560386938</v>
+        <v>11.32736561242285</v>
       </c>
       <c r="F55">
-        <v>1.542226926005428</v>
+        <v>1.751157443583415</v>
       </c>
       <c r="G55">
-        <v>0.01611181163454449</v>
+        <v>0.1191081901732474</v>
       </c>
       <c r="H55">
-        <v>0.1511342340755035</v>
+        <v>0.1362161831649027</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -1879,25 +1879,25 @@
         <v>5.5625</v>
       </c>
       <c r="B56">
-        <v>0.009999997401631506</v>
+        <v>0.009999998030480454</v>
       </c>
       <c r="C56">
-        <v>0.2672777153950399</v>
+        <v>0.2662382065872326</v>
       </c>
       <c r="D56">
-        <v>2.478471076382211</v>
+        <v>2.412114230720801</v>
       </c>
       <c r="E56">
-        <v>12.66197665387967</v>
+        <v>12.01592075379021</v>
       </c>
       <c r="F56">
-        <v>1.618089982553224</v>
+        <v>1.828387383524513</v>
       </c>
       <c r="G56">
-        <v>0.01583802581822729</v>
+        <v>0.1172719374652236</v>
       </c>
       <c r="H56">
-        <v>0.1506837733007752</v>
+        <v>0.1360468638125231</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -1905,25 +1905,25 @@
         <v>5.666666666666667</v>
       </c>
       <c r="B57">
-        <v>0.009999997401631506</v>
+        <v>0.009999998030480454</v>
       </c>
       <c r="C57">
-        <v>0.2683193817910432</v>
+        <v>0.267279873048741</v>
       </c>
       <c r="D57">
-        <v>2.505231782203849</v>
+        <v>2.434441210125876</v>
       </c>
       <c r="E57">
-        <v>13.32173517158563</v>
+        <v>12.6964509137568</v>
       </c>
       <c r="F57">
-        <v>1.694519843078482</v>
+        <v>1.906161256531815</v>
       </c>
       <c r="G57">
-        <v>0.01557308313140421</v>
+        <v>0.1154942901364457</v>
       </c>
       <c r="H57">
-        <v>0.1501901875554356</v>
+        <v>0.1358202747020674</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -1931,25 +1931,25 @@
         <v>5.770833333333334</v>
       </c>
       <c r="B58">
-        <v>0.009999997401625684</v>
+        <v>0.009999998027324703</v>
       </c>
       <c r="C58">
-        <v>0.2693610481870459</v>
+        <v>0.2683215395099207</v>
       </c>
       <c r="D58">
-        <v>2.532184669781635</v>
+        <v>2.456947996891808</v>
       </c>
       <c r="E58">
-        <v>13.97372481743468</v>
+        <v>13.36909851112797</v>
       </c>
       <c r="F58">
-        <v>1.771496542886115</v>
+        <v>1.984451916317726</v>
       </c>
       <c r="G58">
-        <v>0.01531617633953714</v>
+        <v>0.1137687461428668</v>
       </c>
       <c r="H58">
-        <v>0.1496618253069373</v>
+        <v>0.135546912905712</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -1957,25 +1957,25 @@
         <v>5.875</v>
       </c>
       <c r="B59">
-        <v>0.009999997401625684</v>
+        <v>0.009999998027324703</v>
       </c>
       <c r="C59">
-        <v>0.2704027145830487</v>
+        <v>0.2693632059711003</v>
       </c>
       <c r="D59">
-        <v>2.559321084105661</v>
+        <v>2.479624505767529</v>
       </c>
       <c r="E59">
-        <v>14.6180612197708</v>
+        <v>14.03399414764652</v>
       </c>
       <c r="F59">
-        <v>1.849003304421056</v>
+        <v>2.06323691255261</v>
       </c>
       <c r="G59">
-        <v>0.0150666431269834</v>
+        <v>0.1120901380461353</v>
       </c>
       <c r="H59">
-        <v>0.1491054119848035</v>
+        <v>0.1352351409816943</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -1983,25 +1983,25 @@
         <v>5.979166666666667</v>
       </c>
       <c r="B60">
-        <v>0.009999997401625684</v>
+        <v>0.009999998027324703</v>
       </c>
       <c r="C60">
-        <v>0.2714443809790513</v>
+        <v>0.27040487243228</v>
       </c>
       <c r="D60">
-        <v>2.58663362804304</v>
+        <v>2.502462203956765</v>
       </c>
       <c r="E60">
-        <v>15.25485273997982</v>
+        <v>14.6912587405796</v>
       </c>
       <c r="F60">
-        <v>1.92702602478044</v>
+        <v>2.142497550715608</v>
       </c>
       <c r="G60">
-        <v>0.01482393286627266</v>
+        <v>0.1104542894788912</v>
       </c>
       <c r="H60">
-        <v>0.1485264170371018</v>
+        <v>0.1348916956977609</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -2009,25 +2009,25 @@
         <v>6.083333333333334</v>
       </c>
       <c r="B61">
-        <v>0.009999997401625684</v>
+        <v>0.009999998027324703</v>
       </c>
       <c r="C61">
-        <v>0.272486047375054</v>
+        <v>0.2714465388934596</v>
       </c>
       <c r="D61">
-        <v>2.6141159275329</v>
+        <v>2.52545381685045</v>
       </c>
       <c r="E61">
-        <v>15.88420172558275</v>
+        <v>15.34100516340988</v>
       </c>
       <c r="F61">
-        <v>2.005552773551398</v>
+        <v>2.22221817332153</v>
       </c>
       <c r="G61">
-        <v>0.01458757904645624</v>
+        <v>0.1088577726255603</v>
       </c>
       <c r="H61">
-        <v>0.1479293214665728</v>
+        <v>0.1345220579935409</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -2035,25 +2035,25 @@
         <v>6.1875</v>
       </c>
       <c r="B62">
-        <v>0.009999997401654599</v>
+        <v>0.009999998036168146</v>
       </c>
       <c r="C62">
-        <v>0.2735277137710597</v>
+        <v>0.2724882053555604</v>
       </c>
       <c r="D62">
-        <v>2.641762458769941</v>
+        <v>2.548593099311788</v>
       </c>
       <c r="E62">
-        <v>16.50620533555757</v>
+        <v>15.98333953561359</v>
       </c>
       <c r="F62">
-        <v>2.08457342117196</v>
+        <v>2.302385602208279</v>
       </c>
       <c r="G62">
-        <v>0.01435718243624759</v>
+        <v>0.1072977337185864</v>
       </c>
       <c r="H62">
-        <v>0.1473178242395368</v>
+        <v>0.1341307264468237</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2061,25 +2061,25 @@
         <v>6.291666666666667</v>
       </c>
       <c r="B63">
-        <v>0.009999997401654599</v>
+        <v>0.009999998036168146</v>
       </c>
       <c r="C63">
-        <v>0.2745693801670654</v>
+        <v>0.2735298718176612</v>
       </c>
       <c r="D63">
-        <v>2.669568408206976</v>
+        <v>2.57187465758771</v>
       </c>
       <c r="E63">
-        <v>17.1209562348503</v>
+        <v>16.61836221082197</v>
       </c>
       <c r="F63">
-        <v>2.164079338804124</v>
+        <v>2.382988704237762</v>
       </c>
       <c r="G63">
-        <v>0.01413239698847544</v>
+        <v>0.1057717655614022</v>
       </c>
       <c r="H63">
-        <v>0.1466949975205817</v>
+        <v>0.1337214224241122</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2087,25 +2087,25 @@
         <v>6.395833333333334</v>
       </c>
       <c r="B64">
-        <v>0.009999997401654599</v>
+        <v>0.009999998036168146</v>
       </c>
       <c r="C64">
-        <v>0.2756110465630711</v>
+        <v>0.274571538279762</v>
       </c>
       <c r="D64">
-        <v>2.697529569930207</v>
+        <v>2.59529380737246</v>
       </c>
       <c r="E64">
-        <v>17.72854292405361</v>
+        <v>17.24616857799381</v>
       </c>
       <c r="F64">
-        <v>2.24406317414144</v>
+        <v>2.464018045826856</v>
       </c>
       <c r="G64">
-        <v>0.01391291970527704</v>
+        <v>0.1042778127572488</v>
       </c>
       <c r="H64">
-        <v>0.1460634073143278</v>
+        <v>0.1332972460226569</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2113,25 +2113,25 @@
         <v>6.5</v>
       </c>
       <c r="B65">
-        <v>0.009999997401654599</v>
+        <v>0.009999998036168146</v>
       </c>
       <c r="C65">
-        <v>0.2766527129590768</v>
+        <v>0.2756132047418628</v>
       </c>
       <c r="D65">
-        <v>2.725642232833452</v>
+        <v>2.618846460063289</v>
       </c>
       <c r="E65">
-        <v>18.32905067019645</v>
+        <v>17.86684970410115</v>
       </c>
       <c r="F65">
-        <v>2.324518619092821</v>
+        <v>2.54546561638799</v>
       </c>
       <c r="G65">
-        <v>0.01369848230170746</v>
+        <v>0.1028141004177744</v>
       </c>
       <c r="H65">
-        <v>0.1454252066390407</v>
+        <v>0.1328607960624332</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2139,25 +2139,25 @@
         <v>6.604166666666667</v>
       </c>
       <c r="B66">
-        <v>0.009999997401704458</v>
+        <v>0.009999998051735797</v>
       </c>
       <c r="C66">
-        <v>0.2776943793550878</v>
+        <v>0.2766548712055854</v>
       </c>
       <c r="D66">
-        <v>2.753903118014667</v>
+        <v>2.642529030946227</v>
       </c>
       <c r="E66">
-        <v>18.92256164704386</v>
+        <v>18.48049285307895</v>
       </c>
       <c r="F66">
-        <v>2.405440271713701</v>
+        <v>2.627324605268361</v>
       </c>
       <c r="G66">
-        <v>0.01348884542558947</v>
+        <v>0.1013790798319205</v>
       </c>
       <c r="H66">
-        <v>0.1447822100290904</v>
+        <v>0.1324142634398101</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2165,25 +2165,25 @@
         <v>6.708333333333334</v>
       </c>
       <c r="B67">
-        <v>0.009999997401704458</v>
+        <v>0.009999998051735797</v>
       </c>
       <c r="C67">
-        <v>0.2787360457510987</v>
+        <v>0.2776965376693079</v>
       </c>
       <c r="D67">
-        <v>2.782309317376526</v>
+        <v>2.666338363535413</v>
       </c>
       <c r="E67">
-        <v>19.50915524739348</v>
+        <v>19.08718192706224</v>
       </c>
       <c r="F67">
-        <v>2.486823505230213</v>
+        <v>2.70958921852066</v>
       </c>
       <c r="G67">
-        <v>0.01328379365163674</v>
+        <v>0.09997138652263854</v>
       </c>
       <c r="H67">
-        <v>0.1441359520559198</v>
+        <v>0.1319595044875687</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2191,25 +2191,25 @@
         <v>6.8125</v>
       </c>
       <c r="B68">
-        <v>0.009999997401704458</v>
+        <v>0.009999998051735797</v>
       </c>
       <c r="C68">
-        <v>0.2797777121471096</v>
+        <v>0.2787382041330304</v>
       </c>
       <c r="D68">
-        <v>2.81085824103761</v>
+        <v>2.69027166825594</v>
       </c>
       <c r="E68">
-        <v>20.08890839716338</v>
+        <v>19.68699781563636</v>
       </c>
       <c r="F68">
-        <v>2.568664357072736</v>
+        <v>2.792254530218341</v>
       </c>
       <c r="G68">
-        <v>0.01308313146841944</v>
+        <v>0.09858980765509003</v>
       </c>
       <c r="H68">
-        <v>0.1434877341575337</v>
+        <v>0.1314980991793151</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2217,25 +2217,25 @@
         <v>6.916666666666667</v>
       </c>
       <c r="B69">
-        <v>0.009999997401704458</v>
+        <v>0.009999998051735797</v>
       </c>
       <c r="C69">
-        <v>0.2808193785431205</v>
+        <v>0.2797798705967527</v>
       </c>
       <c r="D69">
-        <v>2.839547579356303</v>
+        <v>2.714326471163847</v>
       </c>
       <c r="E69">
-        <v>20.66189562982222</v>
+        <v>20.28001869591048</v>
       </c>
       <c r="F69">
-        <v>2.650959445114161</v>
+        <v>2.875316358476874</v>
       </c>
       <c r="G69">
-        <v>0.01288668110315643</v>
+        <v>0.097233256280103</v>
       </c>
       <c r="H69">
-        <v>0.1428386640740955</v>
+        <v>0.1310313976890784</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2243,25 +2243,25 @@
         <v>7.020833333333334</v>
       </c>
       <c r="B70">
-        <v>0.009999997401769389</v>
+        <v>0.009999998071742787</v>
       </c>
       <c r="C70">
-        <v>0.2818610449391382</v>
+        <v>0.2808215370625594</v>
       </c>
       <c r="D70">
-        <v>2.868375262636448</v>
+        <v>2.738500571349512</v>
       </c>
       <c r="E70">
-        <v>21.22818941222065</v>
+        <v>20.8663202819666</v>
       </c>
       <c r="F70">
-        <v>2.733705884829245</v>
+        <v>2.958771162517477</v>
       </c>
       <c r="G70">
-        <v>0.01269427880929029</v>
+        <v>0.09590075093608731</v>
       </c>
       <c r="H70">
-        <v>0.1421896849498409</v>
+        <v>0.1305605579478553</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2269,25 +2269,25 @@
         <v>7.125</v>
       </c>
       <c r="B71">
-        <v>0.009999997401769389</v>
+        <v>0.009999998071742787</v>
       </c>
       <c r="C71">
-        <v>0.2829027113351558</v>
+        <v>0.2818632035283659</v>
       </c>
       <c r="D71">
-        <v>2.897339432154737</v>
+        <v>2.762792006064253</v>
       </c>
       <c r="E71">
-        <v>21.78786026609448</v>
+        <v>21.44597599534016</v>
       </c>
       <c r="F71">
-        <v>2.81690122703223</v>
+        <v>3.042615957557413</v>
       </c>
       <c r="G71">
-        <v>0.01250577364249178</v>
+        <v>0.09459139938785849</v>
       </c>
       <c r="H71">
-        <v>0.141541601894131</v>
+        <v>0.1300865761801081</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2295,25 +2295,25 @@
         <v>7.229166666666667</v>
       </c>
       <c r="B72">
-        <v>0.009999997401769389</v>
+        <v>0.009999998071742787</v>
       </c>
       <c r="C72">
-        <v>0.2839443777311735</v>
+        <v>0.2829048699941724</v>
       </c>
       <c r="D72">
-        <v>2.926438414372368</v>
+        <v>2.787199018068572</v>
       </c>
       <c r="E72">
-        <v>22.34097690856749</v>
+        <v>22.01905724621179</v>
       </c>
       <c r="F72">
-        <v>2.900543403270591</v>
+        <v>3.126848238525259</v>
       </c>
       <c r="G72">
-        <v>0.01232102563455499</v>
+        <v>0.09330438508215176</v>
       </c>
       <c r="H72">
-        <v>0.1408951026447176</v>
+        <v>0.1296103118007501</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2321,25 +2321,25 @@
         <v>7.333333333333334</v>
       </c>
       <c r="B73">
-        <v>0.009999997401769389</v>
+        <v>0.009999998071742787</v>
       </c>
       <c r="C73">
-        <v>0.2849860441271911</v>
+        <v>0.283946536459979</v>
       </c>
       <c r="D73">
-        <v>2.955670698896542</v>
+        <v>2.811720031431049</v>
       </c>
       <c r="E73">
-        <v>22.88760637427055</v>
+        <v>22.58563353703687</v>
       </c>
       <c r="F73">
-        <v>2.984630679229664</v>
+        <v>3.211465920625113</v>
       </c>
       <c r="G73">
-        <v>0.0121399044337753</v>
+        <v>0.09203895669313093</v>
       </c>
       <c r="H73">
-        <v>0.1402507749232019</v>
+        <v>0.1291325080097299</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2347,25 +2347,25 @@
         <v>7.4375</v>
       </c>
       <c r="B74">
-        <v>0.009999997401846702</v>
+        <v>0.009999998095061986</v>
       </c>
       <c r="C74">
-        <v>0.2860277105232168</v>
+        <v>0.2849882029282146</v>
       </c>
       <c r="D74">
-        <v>2.985034919555201</v>
+        <v>2.836353629309154</v>
       </c>
       <c r="E74">
-        <v>23.42781412217925</v>
+        <v>23.14577261604812</v>
       </c>
       <c r="F74">
-        <v>3.069161614781504</v>
+        <v>3.296467286421402</v>
       </c>
       <c r="G74">
-        <v>0.0119622881722322</v>
+        <v>0.09079441904901042</v>
       </c>
       <c r="H74">
-        <v>0.1396091209023473</v>
+        <v>0.1286538087829993</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2373,25 +2373,25 @@
         <v>7.541666666666667</v>
       </c>
       <c r="B75">
-        <v>0.009999997401846702</v>
+        <v>0.009999998095061986</v>
       </c>
       <c r="C75">
-        <v>0.2870693769192426</v>
+        <v>0.2860298693964502</v>
       </c>
       <c r="D75">
-        <v>3.014529838071484</v>
+        <v>2.861098536147941</v>
       </c>
       <c r="E75">
-        <v>23.96166412961345</v>
+        <v>23.69954054375695</v>
       </c>
       <c r="F75">
-        <v>3.154135029575772</v>
+        <v>3.381850941927913</v>
       </c>
       <c r="G75">
-        <v>0.01178806251531888</v>
+        <v>0.08957012636599955</v>
       </c>
       <c r="H75">
-        <v>0.1389705693267936</v>
+        <v>0.1281747731178067</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2399,25 +2399,25 @@
         <v>7.645833333333334</v>
       </c>
       <c r="B76">
-        <v>0.009999997401846702</v>
+        <v>0.009999998095061986</v>
       </c>
       <c r="C76">
-        <v>0.2881110433152683</v>
+        <v>0.2870715358646858</v>
       </c>
       <c r="D76">
-        <v>3.044154329919261</v>
+        <v>2.885953600600074</v>
       </c>
       <c r="E76">
-        <v>24.48921897548027</v>
+        <v>24.24700184413253</v>
       </c>
       <c r="F76">
-        <v>3.23954997327608</v>
+        <v>3.467615776863171</v>
       </c>
       <c r="G76">
-        <v>0.01161711985869102</v>
+        <v>0.08836547543211415</v>
       </c>
       <c r="H76">
-        <v>0.1383354857157776</v>
+        <v>0.1276958868136562</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -2425,25 +2425,25 @@
         <v>7.75</v>
       </c>
       <c r="B77">
-        <v>0.009999997401846702</v>
+        <v>0.009999998095061986</v>
       </c>
       <c r="C77">
-        <v>0.289152709711294</v>
+        <v>0.2881132023329214</v>
       </c>
       <c r="D77">
-        <v>3.073907372018923</v>
+        <v>2.910917781802074</v>
       </c>
       <c r="E77">
-        <v>25.01053991434622</v>
+        <v>24.78821958249346</v>
       </c>
       <c r="F77">
-        <v>3.325405699710892</v>
+        <v>3.55376093154926</v>
       </c>
       <c r="G77">
-        <v>0.01144935864523941</v>
+        <v>0.08717990099257006</v>
       </c>
       <c r="H77">
-        <v>0.1377041809893875</v>
+        <v>0.1272175725060311</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -2451,25 +2451,25 @@
         <v>7.854166666666667</v>
       </c>
       <c r="B78">
-        <v>0.009999997401935237</v>
+        <v>0.009999998121095078</v>
       </c>
       <c r="C78">
-        <v>0.290194376107329</v>
+        <v>0.2891548688038689</v>
       </c>
       <c r="D78">
-        <v>3.103788031992031</v>
+        <v>2.93599013719534</v>
       </c>
       <c r="E78">
-        <v>25.52568694273506</v>
+        <v>25.32325544912637</v>
       </c>
       <c r="F78">
-        <v>3.411701644337186</v>
+        <v>3.6402857679131</v>
       </c>
       <c r="G78">
-        <v>0.01128468278013215</v>
+        <v>0.08601287136938708</v>
       </c>
       <c r="H78">
-        <v>0.1370769187917516</v>
+        <v>0.126740198096249</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -2477,25 +2477,25 @@
         <v>7.958333333333334</v>
       </c>
       <c r="B79">
-        <v>0.009999997401935237</v>
+        <v>0.009999998121095078</v>
       </c>
       <c r="C79">
-        <v>0.291236042503364</v>
+        <v>0.2901965352748163</v>
       </c>
       <c r="D79">
-        <v>3.133795473429746</v>
+        <v>2.96116981201541</v>
       </c>
       <c r="E79">
-        <v>26.03471776711097</v>
+        <v>25.85216982562311</v>
       </c>
       <c r="F79">
-        <v>3.498437409332444</v>
+        <v>3.727189844385752</v>
       </c>
       <c r="G79">
-        <v>0.01112300105853971</v>
+        <v>0.08486388482954163</v>
       </c>
       <c r="H79">
-        <v>0.1364539221452772</v>
+        <v>0.1262640839186006</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -2503,25 +2503,25 @@
         <v>8.0625</v>
       </c>
       <c r="B80">
-        <v>0.009999997401935237</v>
+        <v>0.009999998121095078</v>
       </c>
       <c r="C80">
-        <v>0.2922777088993989</v>
+        <v>0.2912382017457638</v>
       </c>
       <c r="D80">
-        <v>3.163928904019717</v>
+        <v>2.986456030161174</v>
       </c>
       <c r="E80">
-        <v>26.53769103983207</v>
+        <v>26.37502183798414</v>
       </c>
       <c r="F80">
-        <v>3.58561273045245</v>
+        <v>3.814472893819083</v>
       </c>
       <c r="G80">
-        <v>0.01096422694748853</v>
+        <v>0.08373246655334821</v>
       </c>
       <c r="H80">
-        <v>0.1358353776257983</v>
+        <v>0.1257895088590938</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -2529,25 +2529,25 @@
         <v>8.166666666666668</v>
       </c>
       <c r="B81">
-        <v>0.009999997401935237</v>
+        <v>0.009999998121095078</v>
       </c>
       <c r="C81">
-        <v>0.2933193752954338</v>
+        <v>0.2922798682167111</v>
       </c>
       <c r="D81">
-        <v>3.194187611286113</v>
+        <v>3.011848086046</v>
       </c>
       <c r="E81">
-        <v>27.03466332010952</v>
+        <v>26.89186941132964</v>
       </c>
       <c r="F81">
-        <v>3.673227478845092</v>
+        <v>3.902134804073522</v>
       </c>
       <c r="G81">
-        <v>0.01080827797448601</v>
+        <v>0.08261816601706699</v>
       </c>
       <c r="H81">
-        <v>0.1352214410349771</v>
+        <v>0.1253167155868583</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -2555,25 +2555,25 @@
         <v>8.270833333333334</v>
       </c>
       <c r="B82">
-        <v>0.009999997402034678</v>
+        <v>0.009999998149515724</v>
       </c>
       <c r="C82">
-        <v>0.2943610416914791</v>
+        <v>0.2933215346906191</v>
       </c>
       <c r="D82">
-        <v>3.224570941971009</v>
+        <v>3.037345336716208</v>
       </c>
       <c r="E82">
-        <v>27.52569011699071</v>
+        <v>27.4027693862429</v>
       </c>
       <c r="F82">
-        <v>3.761281641543103</v>
+        <v>3.990175601075471</v>
       </c>
       <c r="G82">
-        <v>0.01065507548112968</v>
+        <v>0.08152055451315669</v>
       </c>
       <c r="H82">
-        <v>0.1346122410168427</v>
+        <v>0.124845914994066</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2581,25 +2581,25 @@
         <v>8.375</v>
       </c>
       <c r="B83">
-        <v>0.009999997402034678</v>
+        <v>0.009999998149515724</v>
       </c>
       <c r="C83">
-        <v>0.2954027080875244</v>
+        <v>0.2943632011645269</v>
       </c>
       <c r="D83">
-        <v>3.255078296286618</v>
+        <v>3.062947196113126</v>
       </c>
       <c r="E83">
-        <v>28.01082593012414</v>
+        <v>27.907777520145</v>
       </c>
       <c r="F83">
-        <v>3.849775309512209</v>
+        <v>4.078595434109379</v>
       </c>
       <c r="G83">
-        <v>0.01050454432691257</v>
+        <v>0.08043922340045996</v>
       </c>
       <c r="H83">
-        <v>0.1340078824624865</v>
+        <v>0.1243772901064048</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -2607,25 +2607,25 @@
         <v>8.479166666666668</v>
       </c>
       <c r="B84">
-        <v>0.009999997402034678</v>
+        <v>0.009999998149515724</v>
       </c>
       <c r="C84">
-        <v>0.2964443744835696</v>
+        <v>0.2954048676384348</v>
       </c>
       <c r="D84">
-        <v>3.285709122794411</v>
+        <v>3.088653129365509</v>
       </c>
       <c r="E84">
-        <v>28.49012428729591</v>
+        <v>28.4069485380347</v>
       </c>
       <c r="F84">
-        <v>3.938708667022537</v>
+        <v>4.167394562475367</v>
       </c>
       <c r="G84">
-        <v>0.01035661263000787</v>
+        <v>0.07937378232336294</v>
       </c>
       <c r="H84">
-        <v>0.1334084494637252</v>
+        <v>0.1239109994185425</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -2633,25 +2633,25 @@
         <v>8.583333333333334</v>
       </c>
       <c r="B85">
-        <v>0.009999997402034678</v>
+        <v>0.009999998149515724</v>
       </c>
       <c r="C85">
-        <v>0.2974860408796149</v>
+        <v>0.2964465341123428</v>
       </c>
       <c r="D85">
-        <v>3.316462913617029</v>
+        <v>3.114462647826141</v>
       </c>
       <c r="E85">
-        <v>28.9636378024942</v>
+        <v>28.9003361704962</v>
       </c>
       <c r="F85">
-        <v>4.028081982322533</v>
+        <v>4.256573343795695</v>
       </c>
       <c r="G85">
-        <v>0.01021121149484128</v>
+        <v>0.07832385771486287</v>
       </c>
       <c r="H85">
-        <v>0.1328140078014906</v>
+        <v>0.1234471797961252</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -2659,25 +2659,25 @@
         <v>8.6875</v>
       </c>
       <c r="B86">
-        <v>0.009999997402145253</v>
+        <v>0.009999998180151121</v>
       </c>
       <c r="C86">
-        <v>0.2985277072756716</v>
+        <v>0.2974882005894419</v>
       </c>
       <c r="D86">
-        <v>3.347339200965437</v>
+        <v>3.140375304404436</v>
       </c>
       <c r="E86">
-        <v>29.43141814036725</v>
+        <v>29.3879932159493</v>
       </c>
       <c r="F86">
-        <v>4.117895598748667</v>
+        <v>4.346132223758556</v>
       </c>
       <c r="G86">
-        <v>0.01006827496723638</v>
+        <v>0.07728909132540544</v>
       </c>
       <c r="H86">
-        <v>0.132224607464485</v>
+        <v>0.1229859489715944</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2685,25 +2685,25 @@
         <v>8.791666666666668</v>
       </c>
       <c r="B87">
-        <v>0.009999997402145253</v>
+        <v>0.009999998180151121</v>
       </c>
       <c r="C87">
-        <v>0.2995693736717284</v>
+        <v>0.2985298670665409</v>
       </c>
       <c r="D87">
-        <v>3.378337552862048</v>
+        <v>3.166390690216663</v>
       </c>
       <c r="E87">
-        <v>29.89351610965527</v>
+        <v>29.86997150207494</v>
       </c>
       <c r="F87">
-        <v>4.208149927496067</v>
+        <v>4.436071726320578</v>
       </c>
       <c r="G87">
-        <v>0.00992773962017616</v>
+        <v>0.07626913967171298</v>
       </c>
       <c r="H87">
-        <v>0.1316402842103947</v>
+        <v>0.1225274078397218</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -2711,25 +2711,25 @@
         <v>8.895833333333334</v>
       </c>
       <c r="B88">
-        <v>0.009999997402145253</v>
+        <v>0.009999998180151121</v>
       </c>
       <c r="C88">
-        <v>0.3006110400677852</v>
+        <v>0.29957153354364</v>
       </c>
       <c r="D88">
-        <v>3.409457570011215</v>
+        <v>3.192508430411881</v>
       </c>
       <c r="E88">
-        <v>30.34998167149665</v>
+        <v>30.34632198638354</v>
       </c>
       <c r="F88">
-        <v>4.298845440679231</v>
+        <v>4.526392445814802</v>
       </c>
       <c r="G88">
-        <v>0.009789544532126999</v>
+        <v>0.07526367213848786</v>
       </c>
       <c r="H88">
-        <v>0.1310610615064584</v>
+        <v>0.1220716422643894</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -2737,25 +2737,25 @@
         <v>9</v>
       </c>
       <c r="B89">
-        <v>0.009999997402145253</v>
+        <v>0.009999998180151121</v>
       </c>
       <c r="C89">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D89">
-        <v>3.440698882807301</v>
+        <v>3.218728181156409</v>
       </c>
       <c r="E89">
-        <v>30.80086396557505</v>
+        <v>30.81709476435828</v>
       </c>
       <c r="F89">
-        <v>4.38998266518026</v>
+        <v>4.617095039366146</v>
       </c>
       <c r="G89">
-        <v>0.009653631102599517</v>
+        <v>0.07427237061746446</v>
       </c>
       <c r="H89">
-        <v>0.130486951972186</v>
+        <v>0.1216187248300636</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -2766,22 +2766,22 @@
         <v>0</v>
       </c>
       <c r="C90">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D90">
-        <v>3.4823579210893</v>
+        <v>3.25483397596121</v>
       </c>
       <c r="E90">
-        <v>30.50310182329531</v>
+        <v>30.53598390377133</v>
       </c>
       <c r="F90">
-        <v>4.492872798125797</v>
+        <v>4.720327138899729</v>
       </c>
       <c r="G90">
-        <v>0.009481254476662137</v>
+        <v>0.07297883944096561</v>
       </c>
       <c r="H90">
-        <v>0.1302117351195284</v>
+        <v>0.1214786939397248</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -2792,22 +2792,22 @@
         <v>0</v>
       </c>
       <c r="C91">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D91">
-        <v>3.5244245010452</v>
+        <v>3.291298390298614</v>
       </c>
       <c r="E91">
-        <v>30.20276424374489</v>
+        <v>30.25232575096638</v>
       </c>
       <c r="F91">
-        <v>4.597033919019196</v>
+        <v>4.824796506627058</v>
       </c>
       <c r="G91">
-        <v>0.009311510173911065</v>
+        <v>0.07169428344985473</v>
       </c>
       <c r="H91">
-        <v>0.1299390390628261</v>
+        <v>0.121338423177521</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -2818,22 +2818,22 @@
         <v>0</v>
       </c>
       <c r="C92">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D92">
-        <v>3.566902432754979</v>
+        <v>3.328124721793656</v>
       </c>
       <c r="E92">
-        <v>29.8998265380061</v>
+        <v>29.96609645197695</v>
       </c>
       <c r="F92">
-        <v>4.70247833150728</v>
+        <v>4.930515001890269</v>
       </c>
       <c r="G92">
-        <v>0.009144442304736664</v>
+        <v>0.0704265953596425</v>
       </c>
       <c r="H92">
-        <v>0.1296689084427452</v>
+        <v>0.1211986529654005</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -2844,22 +2844,22 @@
         <v>0</v>
       </c>
       <c r="C93">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D93">
-        <v>3.609795260637695</v>
+        <v>3.365316140573206</v>
       </c>
       <c r="E93">
-        <v>29.59426564686886</v>
+        <v>29.6772729904847</v>
       </c>
       <c r="F93">
-        <v>4.809217541784257</v>
+        <v>5.037494052989334</v>
       </c>
       <c r="G93">
-        <v>0.008979998441968774</v>
+        <v>0.06917552440839739</v>
       </c>
       <c r="H93">
-        <v>0.1294012335351686</v>
+        <v>0.1210593190730354</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -2870,22 +2870,22 @@
         <v>0</v>
       </c>
       <c r="C94">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D94">
-        <v>3.653106530195182</v>
+        <v>3.402875819929836</v>
       </c>
       <c r="E94">
-        <v>29.28605845620666</v>
+        <v>29.38583228335194</v>
       </c>
       <c r="F94">
-        <v>4.91726309005368</v>
+        <v>5.145745125534579</v>
       </c>
       <c r="G94">
-        <v>0.008818127602138131</v>
+        <v>0.06794082497354578</v>
       </c>
       <c r="H94">
-        <v>0.1291359036097816</v>
+        <v>0.1209203555756269</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -2896,22 +2896,22 @@
         <v>0</v>
       </c>
       <c r="C95">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D95">
-        <v>3.696839785924653</v>
+        <v>3.440806934686811</v>
       </c>
       <c r="E95">
-        <v>28.97518180718937</v>
+        <v>29.09175118969625</v>
       </c>
       <c r="F95">
-        <v>5.026626545940141</v>
+        <v>5.255279718396618</v>
       </c>
       <c r="G95">
-        <v>0.008658780186496165</v>
+        <v>0.06672225647354753</v>
       </c>
       <c r="H95">
-        <v>0.1288728066943435</v>
+        <v>0.1207816947049405</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -2922,22 +2922,22 @@
         <v>0</v>
       </c>
       <c r="C96">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D96">
-        <v>3.740998569062461</v>
+        <v>3.479112659434053</v>
       </c>
       <c r="E96">
-        <v>28.66161250735146</v>
+        <v>28.79500652070699</v>
       </c>
       <c r="F96">
-        <v>5.137319503510104</v>
+        <v>5.366109359317309</v>
       </c>
       <c r="G96">
-        <v>0.008501907940672966</v>
+        <v>0.06551958327172892</v>
       </c>
       <c r="H96">
-        <v>0.1286118293518095</v>
+        <v>0.1206432666887164</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -2948,22 +2948,22 @@
         <v>0</v>
       </c>
       <c r="C97">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D97">
-        <v>3.785586415144633</v>
+        <v>3.517796166624591</v>
       </c>
       <c r="E97">
-        <v>28.34532734258837</v>
+        <v>28.4955750502642</v>
       </c>
       <c r="F97">
-        <v>5.249353575868497</v>
+        <v>5.47824560015419</v>
       </c>
       <c r="G97">
-        <v>0.008347463916234258</v>
+        <v>0.0643325745845675</v>
       </c>
       <c r="H97">
-        <v>0.1283528564425332</v>
+        <v>0.1205049995775463</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -2974,22 +2974,22 @@
         <v>0</v>
       </c>
       <c r="C98">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D98">
-        <v>3.830606851368431</v>
+        <v>3.556860624519959</v>
       </c>
       <c r="E98">
-        <v>28.0263030901606</v>
+        <v>28.19343352642604</v>
       </c>
       <c r="F98">
-        <v>5.36274038929476</v>
+        <v>5.591700011728301</v>
       </c>
       <c r="G98">
-        <v>0.008195402434087552</v>
+        <v>0.0631610043944493</v>
       </c>
       <c r="H98">
-        <v>0.1280957708698581</v>
+        <v>0.1203668190579558</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -3000,22 +3000,22 @@
         <v>0</v>
       </c>
       <c r="C99">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D99">
-        <v>3.876063393737617</v>
+        <v>3.596309194971946</v>
       </c>
       <c r="E99">
-        <v>27.70451653279338</v>
+        <v>27.88855868385718</v>
       </c>
       <c r="F99">
-        <v>5.477491576878349</v>
+        <v>5.706484178242314</v>
       </c>
       <c r="G99">
-        <v>0.008045679049693923</v>
+        <v>0.0620046513669336</v>
       </c>
       <c r="H99">
-        <v>0.1278404533072063</v>
+        <v>0.1202286482502893</v>
       </c>
     </row>
     <row r="100" spans="1:8">
@@ -3026,22 +3026,22 @@
         <v>0</v>
       </c>
       <c r="C100">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D100">
-        <v>3.921959543972297</v>
+        <v>3.636145031026809</v>
       </c>
       <c r="E100">
-        <v>27.37994447396825</v>
+        <v>27.58092725727797</v>
       </c>
       <c r="F100">
-        <v>5.593618771609653</v>
+        <v>5.822609691232722</v>
       </c>
       <c r="G100">
-        <v>0.00789825052004858</v>
+        <v>0.06086329877258139</v>
       </c>
       <c r="H100">
-        <v>0.127586781904556</v>
+        <v>0.120090407489831</v>
       </c>
     </row>
     <row r="101" spans="1:8">
@@ -3052,22 +3052,22 @@
         <v>0</v>
       </c>
       <c r="C101">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D101">
-        <v>3.968298786162269</v>
+        <v>3.67637127433673</v>
       </c>
       <c r="E101">
-        <v>27.05256375451314</v>
+        <v>27.2705159960217</v>
       </c>
       <c r="F101">
-        <v>5.711133598877736</v>
+        <v>5.940088143016252</v>
       </c>
       <c r="G101">
-        <v>0.007753074772400209</v>
+        <v>0.059736734413422</v>
       </c>
       <c r="H101">
-        <v>0.1273346319719475</v>
+        <v>0.1199520140894137</v>
       </c>
     </row>
     <row r="102" spans="1:8">
@@ -3078,22 +3078,22 @@
         <v>0</v>
       </c>
       <c r="C102">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D102">
-        <v>4.015084583140579</v>
+        <v>3.716991052361725</v>
       </c>
       <c r="E102">
-        <v>26.72235127060864</v>
+        <v>26.95730167979628</v>
       </c>
       <c r="F102">
-        <v>5.830047668321267</v>
+        <v>6.058931119586662</v>
       </c>
       <c r="G102">
-        <v>0.007610110874686196</v>
+        <v>0.05862475055415596</v>
       </c>
       <c r="H102">
-        <v>0.127083875637372</v>
+        <v>0.1198133820815587</v>
       </c>
     </row>
     <row r="103" spans="1:8">
@@ -3104,22 +3104,22 @@
         <v>0</v>
       </c>
       <c r="C103">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D103">
-        <v>4.062320372551477</v>
+        <v>3.758007475343519</v>
       </c>
       <c r="E103">
-        <v>26.38928399334057</v>
+        <v>26.64126113575643</v>
       </c>
       <c r="F103">
-        <v>5.950372564973231</v>
+        <v>6.179150192913598</v>
       </c>
       <c r="G103">
-        <v>0.007469319007668478</v>
+        <v>0.05752714385821611</v>
       </c>
       <c r="H103">
-        <v>0.1268343814760694</v>
+        <v>0.1196744219379556</v>
       </c>
     </row>
     <row r="104" spans="1:8">
@@ -3130,22 +3130,22 @@
         <v>0</v>
       </c>
       <c r="C104">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D104">
-        <v>4.110009562584183</v>
+        <v>3.799423633030953</v>
       </c>
       <c r="E104">
-        <v>26.05333898994322</v>
+        <v>26.32237125700349</v>
       </c>
       <c r="F104">
-        <v>6.0721198396337</v>
+        <v>6.300756912590234</v>
       </c>
       <c r="G104">
-        <v>0.007330660438762747</v>
+        <v>0.05644371532883738</v>
       </c>
       <c r="H104">
-        <v>0.12658601410789</v>
+        <v>0.1195350402638221</v>
       </c>
     </row>
     <row r="105" spans="1:8">
@@ -3156,22 +3156,22 @@
         <v>0</v>
       </c>
       <c r="C105">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D105">
-        <v>4.158155527340705</v>
+        <v>3.841242591134328</v>
       </c>
       <c r="E105">
-        <v>25.71449344689325</v>
+        <v>26.00060902264226</v>
       </c>
       <c r="F105">
-        <v>6.195300998397642</v>
+        <v>6.423762796770773</v>
       </c>
       <c r="G105">
-        <v>0.007194097497562357</v>
+        <v>0.05537427025531538</v>
       </c>
       <c r="H105">
-        <v>0.1263386337589449</v>
+        <v>0.1193951394643775</v>
       </c>
     </row>
     <row r="106" spans="1:8">
@@ -3182,22 +3182,22 @@
         <v>0</v>
       </c>
       <c r="C106">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D106">
-        <v>4.206761601802393</v>
+        <v>3.883467387483724</v>
       </c>
       <c r="E106">
-        <v>25.37272469503234</v>
+        <v>25.67595151953801</v>
       </c>
       <c r="F106">
-        <v>6.319927491256661</v>
+        <v>6.548179322332617</v>
       </c>
       <c r="G106">
-        <v>0.007059593553067783</v>
+        <v>0.05431861816466928</v>
       </c>
       <c r="H106">
-        <v>0.1260920957832788</v>
+        <v>0.1192546173803166</v>
       </c>
     </row>
     <row r="107" spans="1:8">
@@ -3208,22 +3208,22 @@
         <v>0</v>
       </c>
       <c r="C107">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D107">
-        <v>4.255831076355871</v>
+        <v>3.926101027863497</v>
       </c>
       <c r="E107">
-        <v>25.02801023691681</v>
+        <v>25.34837596593261</v>
       </c>
       <c r="F107">
-        <v>6.446010699684338</v>
+        <v>6.674017914190951</v>
       </c>
       <c r="G107">
-        <v>0.006927112992642661</v>
+        <v>0.05327657277896363</v>
       </c>
       <c r="H107">
-        <v>0.1258462501397332</v>
+        <v>0.1191133668887705</v>
       </c>
     </row>
     <row r="108" spans="1:8">
@@ -3234,22 +3234,22 @@
         <v>0</v>
       </c>
       <c r="C108">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D108">
-        <v>4.305367190834454</v>
+        <v>3.969146481492188</v>
       </c>
       <c r="E108">
-        <v>24.68032777661522</v>
+        <v>25.01785973709597</v>
       </c>
       <c r="F108">
-        <v>6.573561923104429</v>
+        <v>6.801289933685508</v>
       </c>
       <c r="G108">
-        <v>0.00679662120272883</v>
+        <v>0.05224795197858615</v>
       </c>
       <c r="H108">
-        <v>0.1256009408185149</v>
+        <v>0.1189712754657838</v>
       </c>
     </row>
     <row r="109" spans="1:8">
@@ -3260,22 +3260,22 @@
         <v>0</v>
       </c>
       <c r="C109">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D109">
-        <v>4.355373128025949</v>
+        <v>4.012606676113546</v>
       </c>
       <c r="E109">
-        <v>24.32965525220122</v>
+        <v>24.68438039320899</v>
       </c>
       <c r="F109">
-        <v>6.702592364129405</v>
+        <v>6.930006665950315</v>
       </c>
       <c r="G109">
-        <v>0.006668084551365487</v>
+        <v>0.05123257777183059</v>
       </c>
       <c r="H109">
-        <v>0.1253560052112316</v>
+        <v>0.1188282247058109</v>
       </c>
     </row>
     <row r="110" spans="1:8">
@@ -3286,22 +3286,22 @@
         <v>0</v>
       </c>
       <c r="C110">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D110">
-        <v>4.405852006591845</v>
+        <v>4.056484492660438</v>
       </c>
       <c r="E110">
-        <v>23.97597087121802</v>
+        <v>24.34791570969642</v>
       </c>
       <c r="F110">
-        <v>6.833113112443299</v>
+        <v>7.060179306167007</v>
       </c>
       <c r="G110">
-        <v>0.006541470372571752</v>
+        <v>0.05023027627118955</v>
       </c>
       <c r="H110">
-        <v>0.1251112734172824</v>
+        <v>0.1186840897931335</v>
       </c>
     </row>
     <row r="111" spans="1:8">
@@ -3312,22 +3312,22 @@
         <v>0</v>
       </c>
       <c r="C111">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D111">
-        <v>4.456806873336195</v>
+        <v>4.100782759448997</v>
       </c>
       <c r="E111">
-        <v>23.61925314942502</v>
+        <v>24.00844371025367</v>
       </c>
       <c r="F111">
-        <v>6.96513512718762</v>
+        <v>7.191818944590818</v>
       </c>
       <c r="G111">
-        <v>0.006416746952667975</v>
+        <v>0.04924087767682647</v>
       </c>
       <c r="H111">
-        <v>0.1248665674784762</v>
+        <v>0.1185387389193986</v>
       </c>
     </row>
     <row r="112" spans="1:8">
@@ -3338,22 +3338,22 @@
         <v>0</v>
       </c>
       <c r="C112">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D112">
-        <v>4.508240694754821</v>
+        <v>4.145504245855257</v>
       </c>
       <c r="E112">
-        <v>23.25948095317516</v>
+        <v>23.66594270283985</v>
       </c>
       <c r="F112">
-        <v>7.098669217691555</v>
+        <v>7.324936550225294</v>
       </c>
       <c r="G112">
-        <v>0.00629388351862946</v>
+        <v>0.04826421626777301</v>
       </c>
       <c r="H112">
-        <v>0.1246217005325758</v>
+        <v>0.1183920326406743</v>
       </c>
     </row>
     <row r="113" spans="1:8">
@@ -3364,22 +3364,22 @@
         <v>0</v>
       </c>
       <c r="C113">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D113">
-        <v>4.560156347786649</v>
+        <v>4.190651655420816</v>
       </c>
       <c r="E113">
-        <v>22.8966335458156</v>
+        <v>23.32039131894297</v>
       </c>
       <c r="F113">
-        <v>7.233726022367724</v>
+        <v>7.459542953006819</v>
       </c>
       <c r="G113">
-        <v>0.006172850228587084</v>
+        <v>0.0473001304014803</v>
       </c>
       <c r="H113">
-        <v>0.1243764758750844</v>
+        <v>0.1182438231664856</v>
       </c>
     </row>
     <row r="114" spans="1:8">
@@ -3390,22 +3390,22 @@
         <v>0</v>
       </c>
       <c r="C114">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D114">
-        <v>4.612556609678952</v>
+        <v>4.236227618327441</v>
       </c>
       <c r="E114">
-        <v>22.53069063855529</v>
+        <v>22.97176855645957</v>
       </c>
       <c r="F114">
-        <v>7.370315985571787</v>
+        <v>7.595648824343208</v>
       </c>
       <c r="G114">
-        <v>0.006053618164613523</v>
+        <v>0.04634846252245545</v>
       </c>
       <c r="H114">
-        <v>0.124130685916986</v>
+        <v>0.1180939535722058</v>
       </c>
     </row>
     <row r="115" spans="1:8">
@@ -3416,22 +3416,22 @@
         <v>0</v>
       </c>
       <c r="C115">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D115">
-        <v>4.665444146866622</v>
+        <v>4.282234683173056</v>
       </c>
       <c r="E115">
-        <v>22.16163244630005</v>
+        <v>22.62005382657453</v>
       </c>
       <c r="F115">
-        <v>7.508449332197893</v>
+        <v>7.733264655831105</v>
       </c>
       <c r="G115">
-        <v>0.005936159327961648</v>
+        <v>0.04540905918082636</v>
       </c>
       <c r="H115">
-        <v>0.1238841110242645</v>
+        <v>0.11794225692492</v>
       </c>
     </row>
     <row r="116" spans="1:8">
@@ -3442,22 +3442,22 @@
         <v>0</v>
       </c>
       <c r="C116">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D116">
-        <v>4.718821502752238</v>
+        <v>4.328675307972958</v>
       </c>
       <c r="E116">
-        <v>21.78943974902374</v>
+        <v>22.26522700507538</v>
       </c>
       <c r="F116">
-        <v>7.648136039751494</v>
+        <v>7.872400735954833</v>
       </c>
       <c r="G116">
-        <v>0.005820446636954075</v>
+        <v>0.04448177106181293</v>
       </c>
       <c r="H116">
-        <v>0.1236365182228081</v>
+        <v>0.1177885553113991</v>
       </c>
     </row>
     <row r="117" spans="1:8">
@@ -3468,22 +3468,22 @@
         <v>0</v>
       </c>
       <c r="C117">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D117">
-        <v>4.772691084258269</v>
+        <v>4.375551850300168</v>
       </c>
       <c r="E117">
-        <v>21.41409395932059</v>
+        <v>21.90726848859149</v>
       </c>
       <c r="F117">
-        <v>7.789385807606012</v>
+        <v>8.013067124543833</v>
       </c>
       <c r="G117">
-        <v>0.005706453927760947</v>
+        <v>0.04356645302723812</v>
       </c>
       <c r="H117">
-        <v>0.1233876597496907</v>
+        <v>0.1176326587551026</v>
       </c>
     </row>
     <row r="118" spans="1:8">
@@ -3494,22 +3494,22 @@
         <v>0</v>
       </c>
       <c r="C118">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D118">
-        <v>4.827055164523957</v>
+        <v>4.422866556467516</v>
       </c>
       <c r="E118">
-        <v>21.03557705252854</v>
+        <v>21.54615925631339</v>
       </c>
       <c r="F118">
-        <v>7.93220809955077</v>
+        <v>8.155273624736539</v>
       </c>
       <c r="G118">
-        <v>0.005594155949404155</v>
+        <v>0.04266296417039282</v>
       </c>
       <c r="H118">
-        <v>0.1231372713534109</v>
+        <v>0.1174743640071001</v>
       </c>
     </row>
     <row r="119" spans="1:8">
@@ -3520,22 +3520,22 @@
         <v>0</v>
       </c>
       <c r="C119">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D119">
-        <v>4.881915813075508</v>
+        <v>4.470621549640885</v>
       </c>
       <c r="E119">
-        <v>20.65387208386869</v>
+        <v>21.1818809378217</v>
       </c>
       <c r="F119">
-        <v>8.076611876692782</v>
+        <v>8.299029752164641</v>
       </c>
       <c r="G119">
-        <v>0.005483528377237586</v>
+        <v>0.04177116788578356</v>
       </c>
       <c r="H119">
-        <v>0.1228850706572177</v>
+        <v>0.1173134531934267</v>
       </c>
     </row>
     <row r="120" spans="1:8">
@@ -3546,22 +3546,22 @@
         <v>0</v>
       </c>
       <c r="C120">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D120">
-        <v>4.937274931798818</v>
+        <v>4.518818816757843</v>
       </c>
       <c r="E120">
-        <v>20.26896284405496</v>
+        <v>20.81441588774162</v>
       </c>
       <c r="F120">
-        <v>8.22260578542631</v>
+        <v>8.444344701032739</v>
       </c>
       <c r="G120">
-        <v>0.005374547864079036</v>
+        <v>0.04089093195554169</v>
       </c>
       <c r="H120">
-        <v>0.1226307549899272</v>
+        <v>0.1171496922985724</v>
       </c>
     </row>
     <row r="121" spans="1:8">
@@ -3572,22 +3572,22 @@
         <v>0</v>
       </c>
       <c r="C121">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D121">
-        <v>4.993134216711558</v>
+        <v>4.567460194108298</v>
       </c>
       <c r="E121">
-        <v>19.880834105096</v>
+        <v>20.44374726803868</v>
       </c>
       <c r="F121">
-        <v>8.370198035301813</v>
+        <v>8.591227306722899</v>
       </c>
       <c r="G121">
-        <v>0.005267191994539865</v>
+        <v>0.04002212865457048</v>
       </c>
       <c r="H121">
-        <v>0.1223739990194</v>
+        <v>0.116982829461488</v>
       </c>
     </row>
     <row r="122" spans="1:8">
@@ -3598,22 +3598,22 @@
         <v>0</v>
       </c>
       <c r="C122">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D122">
-        <v>5.049495135699776</v>
+        <v>4.616547365780955</v>
       </c>
       <c r="E122">
-        <v>19.48947173216383</v>
+        <v>20.06985899285478</v>
       </c>
       <c r="F122">
-        <v>8.519396348104488</v>
+        <v>8.739686082751108</v>
       </c>
       <c r="G122">
-        <v>0.00516143933026627</v>
+        <v>0.03916463475605012</v>
       </c>
       <c r="H122">
-        <v>0.1221144521594787</v>
+        <v>0.116812592979585</v>
       </c>
     </row>
     <row r="123" spans="1:8">
@@ -3624,22 +3624,22 @@
         <v>0</v>
       </c>
       <c r="C123">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D123">
-        <v>5.106358903755017</v>
+        <v>4.666081801289302</v>
       </c>
       <c r="E123">
-        <v>19.09486280800894</v>
+        <v>19.69273627442279</v>
       </c>
       <c r="F123">
-        <v>8.670207901223439</v>
+        <v>8.889728937402451</v>
       </c>
       <c r="G123">
-        <v>0.005057269436199776</v>
+        <v>0.03831833197123251</v>
       </c>
       <c r="H123">
-        <v>0.1218517355793793</v>
+        <v>0.1166386893648151</v>
       </c>
     </row>
     <row r="124" spans="1:8">
@@ -3650,22 +3650,22 @@
         <v>0</v>
       </c>
       <c r="C124">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D124">
-        <v>5.163726455373434</v>
+        <v>4.716064782136079</v>
       </c>
       <c r="E124">
-        <v>18.69699577161485</v>
+        <v>19.31236528371713</v>
       </c>
       <c r="F124">
-        <v>8.822639264542627</v>
+        <v>9.041363362835355</v>
       </c>
       <c r="G124">
-        <v>0.004954662913233579</v>
+        <v>0.03748310702853423</v>
       </c>
       <c r="H124">
-        <v>0.1215854387973517</v>
+        <v>0.1164608006904564</v>
       </c>
     </row>
     <row r="125" spans="1:8">
@@ -3676,22 +3676,22 @@
         <v>0</v>
       </c>
       <c r="C125">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D125">
-        <v>5.221598413723607</v>
+        <v>4.766497364413286</v>
       </c>
       <c r="E125">
-        <v>18.29586057305657</v>
+        <v>18.92873342574874</v>
       </c>
       <c r="F125">
-        <v>8.976696329961349</v>
+        <v>9.19459629846904</v>
       </c>
       <c r="G125">
-        <v>0.004853601438221082</v>
+        <v>0.03665885169765782</v>
       </c>
       <c r="H125">
-        <v>0.121315115789536</v>
+        <v>0.1162785818547058</v>
       </c>
     </row>
     <row r="126" spans="1:8">
@@ -3702,22 +3702,22 @@
         <v>0</v>
       </c>
       <c r="C126">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D126">
-        <v>5.279975055626188</v>
+        <v>4.817380356418441</v>
       </c>
       <c r="E126">
-        <v>17.89144882443968</v>
+        <v>18.54182944459644</v>
       </c>
       <c r="F126">
-        <v>9.132384247448854</v>
+        <v>9.349434087438732</v>
       </c>
       <c r="G126">
-        <v>0.004754067759686537</v>
+        <v>0.03584546288881198</v>
       </c>
       <c r="H126">
-        <v>0.1210402804289678</v>
+        <v>0.1160916573840258</v>
       </c>
     </row>
     <row r="127" spans="1:8">
@@ -3728,22 +3728,22 @@
         <v>0</v>
       </c>
       <c r="C127">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D127">
-        <v>5.338856272477263</v>
+        <v>4.86871428560783</v>
       </c>
       <c r="E127">
-        <v>17.48375406723479</v>
+        <v>18.15164367726381</v>
       </c>
       <c r="F127">
-        <v>9.28970728984298</v>
+        <v>9.505882349171047</v>
       </c>
       <c r="G127">
-        <v>0.004656045966973108</v>
+        <v>0.03504284395473281</v>
       </c>
       <c r="H127">
-        <v>0.1207604017553927</v>
+        <v>0.1158996179798234</v>
       </c>
     </row>
     <row r="128" spans="1:8">
@@ -3754,22 +3754,22 @@
         <v>0</v>
       </c>
       <c r="C128">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D128">
-        <v>5.398241528072885</v>
+        <v>4.920499375289585</v>
       </c>
       <c r="E128">
-        <v>17.07277191585906</v>
+        <v>17.75816812360144</v>
       </c>
       <c r="F128">
-        <v>9.448668800495415</v>
+        <v>9.663945959248521</v>
       </c>
       <c r="G128">
-        <v>0.004559521248523215</v>
+        <v>0.03425090356525774</v>
       </c>
       <c r="H128">
-        <v>0.1204748975086652</v>
+        <v>0.1157020161918504</v>
       </c>
     </row>
     <row r="129" spans="1:8">
@@ -3780,22 +3780,22 @@
         <v>0</v>
       </c>
       <c r="C129">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D129">
-        <v>5.45812980858536</v>
+        <v>4.972735508534686</v>
       </c>
       <c r="E129">
-        <v>16.65850033042774</v>
+        <v>17.36139667237437</v>
       </c>
       <c r="F129">
-        <v>9.60927106504016</v>
+        <v>9.823628942942689</v>
       </c>
       <c r="G129">
-        <v>0.004464480178964074</v>
+        <v>0.0334695570208686</v>
       </c>
       <c r="H129">
-        <v>0.1201831276413095</v>
+        <v>0.1154983617913888</v>
       </c>
     </row>
     <row r="130" spans="1:8">
@@ -3806,22 +3806,22 @@
         <v>0</v>
       </c>
       <c r="C130">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D130">
-        <v>5.518519566832783</v>
+        <v>5.02542219034543</v>
       </c>
       <c r="E130">
-        <v>16.24093989625276</v>
+        <v>16.96132531689761</v>
       </c>
       <c r="F130">
-        <v>9.771515184262334</v>
+        <v>9.984934377245699</v>
       </c>
       <c r="G130">
-        <v>0.004370910769185484</v>
+        <v>0.03269872649244851</v>
       </c>
       <c r="H130">
-        <v>0.1198843863006419</v>
+        <v>0.1152881162993</v>
       </c>
     </row>
     <row r="131" spans="1:8">
@@ -3832,22 +3832,22 @@
         <v>0</v>
       </c>
       <c r="C131">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D131">
-        <v>5.579408659023041</v>
+        <v>5.07855850505514</v>
       </c>
       <c r="E131">
-        <v>15.82009414096251</v>
+        <v>16.55795239777724</v>
       </c>
       <c r="F131">
-        <v>9.935400929877588</v>
+        <v>10.14786428059936</v>
       </c>
       <c r="G131">
-        <v>0.004278802585095825</v>
+        <v>0.03193834155428951</v>
       </c>
       <c r="H131">
-        <v>0.1195778925796578</v>
+        <v>0.1150706866932616</v>
       </c>
     </row>
     <row r="132" spans="1:8">
@@ -3858,22 +3858,22 @@
         <v>0</v>
       </c>
       <c r="C132">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D132">
-        <v>5.64079427658901</v>
+        <v>5.132143068225953</v>
       </c>
       <c r="E132">
-        <v>15.39596988365678</v>
+        <v>16.15127887690677</v>
       </c>
       <c r="F132">
-        <v>10.10092658432682</v>
+        <v>10.31241948844022</v>
       </c>
       <c r="G132">
-        <v>0.004188146884355968</v>
+        <v>0.03118833980800734</v>
       </c>
       <c r="H132">
-        <v>0.1192627796856637</v>
+        <v>0.1148454181180482</v>
       </c>
     </row>
     <row r="133" spans="1:8">
@@ -3884,22 +3884,22 @@
         <v>0</v>
       </c>
       <c r="C133">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D133">
-        <v>5.702672864580543</v>
+        <v>5.186173972471533</v>
       </c>
       <c r="E133">
-        <v>14.96857763912972</v>
+        <v>15.74130864674181</v>
       </c>
       <c r="F133">
-        <v>10.26808875787541</v>
+        <v>10.47859951259385</v>
       </c>
       <c r="G133">
-        <v>0.004098936781619804</v>
+        <v>0.03044866761432617</v>
       </c>
       <c r="H133">
-        <v>0.1189380822189709</v>
+        <v>0.1146115854110435</v>
       </c>
     </row>
     <row r="134" spans="1:8">
@@ -3910,22 +3910,22 @@
         <v>0</v>
       </c>
       <c r="C134">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D134">
-        <v>5.76504001969667</v>
+        <v>5.240648731923617</v>
       </c>
       <c r="E134">
-        <v>14.53793211525737</v>
+        <v>15.32804885934693</v>
       </c>
       <c r="F134">
-        <v>10.43688216503735</v>
+        <v>10.646402389478</v>
       </c>
       <c r="G134">
-        <v>0.004011167467723207</v>
+        <v>0.02971928088526326</v>
       </c>
       <c r="H134">
-        <v>0.1186027212189385</v>
+        <v>0.1143683831999949</v>
       </c>
     </row>
     <row r="135" spans="1:8">
@@ -3936,22 +3936,22 @@
         <v>0</v>
       </c>
       <c r="C135">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D135">
-        <v>5.827890385962445</v>
+        <v>5.295564201733773</v>
       </c>
       <c r="E135">
-        <v>14.10405274507084</v>
+        <v>14.91151035662129</v>
       </c>
       <c r="F135">
-        <v>10.60729938086501</v>
+        <v>10.81582448986249</v>
       </c>
       <c r="G135">
-        <v>0.003924836442750735</v>
+        <v>0.02900014613376446</v>
       </c>
       <c r="H135">
-        <v>0.1182554863876226</v>
+        <v>0.1141149143300349</v>
       </c>
     </row>
     <row r="136" spans="1:8">
@@ -3962,22 +3962,22 @@
         <v>0</v>
       </c>
       <c r="C136">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D136">
-        <v>5.89121752956314</v>
+        <v>5.350916501576075</v>
       </c>
       <c r="E136">
-        <v>13.66696431279486</v>
+        <v>14.49170811924202</v>
       </c>
       <c r="F136">
-        <v>10.77933055650945</v>
+        <v>10.98686031250992</v>
       </c>
       <c r="G136">
-        <v>0.003839943808997101</v>
+        <v>0.02829124177414593</v>
       </c>
       <c r="H136">
-        <v>0.1178950149541309</v>
+        <v>0.113850176253828</v>
       </c>
     </row>
     <row r="137" spans="1:8">
@@ -3988,22 +3988,22 @@
         <v>0</v>
       </c>
       <c r="C137">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D137">
-        <v>5.955013793677392</v>
+        <v>5.406700923284435</v>
       </c>
       <c r="E137">
-        <v>13.22669767955096</v>
+        <v>14.06866179165324</v>
       </c>
       <c r="F137">
-        <v>10.95296308956858</v>
+        <v>11.15950224589617</v>
       </c>
       <c r="G137">
-        <v>0.003756492624485147</v>
+        <v>0.02759255944908851</v>
       </c>
       <c r="H137">
-        <v>0.1175197663946887</v>
+        <v>0.1135730449372223</v>
       </c>
     </row>
     <row r="138" spans="1:8">
@@ -4014,22 +4014,22 @@
         <v>0</v>
       </c>
       <c r="C138">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D138">
-        <v>6.019270217910398</v>
+        <v>5.462911824480108</v>
       </c>
       <c r="E138">
-        <v>12.78329024776415</v>
+        <v>13.64239628639675</v>
       </c>
       <c r="F138">
-        <v>11.12818140135781</v>
+        <v>11.33374029396892</v>
       </c>
       <c r="G138">
-        <v>0.003674489222178613</v>
+        <v>0.02690410573703722</v>
       </c>
       <c r="H138">
-        <v>0.1171279916154934</v>
+        <v>0.113282255780678</v>
       </c>
     </row>
     <row r="139" spans="1:8">
@@ -4040,22 +4040,22 @@
         <v>0</v>
       </c>
       <c r="C139">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D139">
-        <v>6.083976074738457</v>
+        <v>5.519542505580741</v>
       </c>
       <c r="E139">
-        <v>12.33678808094798</v>
+        <v>13.21294248251062</v>
       </c>
       <c r="F139">
-        <v>11.30496601171823</v>
+        <v>11.50956175927734</v>
       </c>
       <c r="G139">
-        <v>0.003593944064250966</v>
+        <v>0.02622590418121434</v>
       </c>
       <c r="H139">
-        <v>0.1167176974520149</v>
+        <v>0.1129763808813572</v>
       </c>
     </row>
     <row r="140" spans="1:8">
@@ -4066,22 +4066,22 @@
         <v>0</v>
       </c>
       <c r="C140">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D140">
-        <v>6.149118861107705</v>
+        <v>5.576585144327277</v>
       </c>
       <c r="E140">
-        <v>11.88724613112246</v>
+        <v>12.78033765706371</v>
       </c>
       <c r="F140">
-        <v>11.48329340030327</v>
+        <v>11.68695103623581</v>
       </c>
       <c r="G140">
-        <v>0.003514872116642603</v>
+        <v>0.02555799684896376</v>
       </c>
       <c r="H140">
-        <v>0.1162866010584626</v>
+        <v>0.1126538014748352</v>
       </c>
     </row>
     <row r="141" spans="1:8">
@@ -4092,22 +4092,22 @@
         <v>0</v>
       </c>
       <c r="C141">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D141">
-        <v>6.214684203611937</v>
+        <v>5.634030397918747</v>
       </c>
       <c r="E141">
-        <v>11.43472876464441</v>
+        <v>12.34462755364962</v>
       </c>
       <c r="F141">
-        <v>11.66313575783179</v>
+        <v>11.86588870753605</v>
       </c>
       <c r="G141">
-        <v>0.003437293410910626</v>
+        <v>0.02490044992919185</v>
       </c>
       <c r="H141">
-        <v>0.115832074184724</v>
+        <v>0.1123126760974726</v>
       </c>
     </row>
     <row r="142" spans="1:8">
@@ -4118,22 +4118,22 @@
         <v>0</v>
       </c>
       <c r="C142">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D142">
-        <v>6.280654998061571</v>
+        <v>5.691867404196057</v>
       </c>
       <c r="E142">
-        <v>10.97931379892149</v>
+        <v>11.90586655495156</v>
       </c>
       <c r="F142">
-        <v>11.8444592029115</v>
+        <v>12.04635143301542</v>
       </c>
       <c r="G142">
-        <v>0.003361234702271059</v>
+        <v>0.0242533550297367</v>
       </c>
       <c r="H142">
-        <v>0.1153510788435994</v>
+        <v>0.1119509001769723</v>
       </c>
     </row>
     <row r="143" spans="1:8">
@@ -4144,22 +4144,22 @@
         <v>0</v>
       </c>
       <c r="C143">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D143">
-        <v>6.347011463462036</v>
+        <v>5.750083701305301</v>
       </c>
       <c r="E143">
-        <v>10.5210924471413</v>
+        <v>11.46411818608299</v>
       </c>
       <c r="F143">
-        <v>12.02722376618662</v>
+        <v>12.22831171267401</v>
       </c>
       <c r="G143">
-        <v>0.003286730163822401</v>
+        <v>0.02361683207672156</v>
       </c>
       <c r="H143">
-        <v>0.1148400816507338</v>
+        <v>0.1115660569214734</v>
       </c>
     </row>
     <row r="144" spans="1:8">
@@ -4170,22 +4170,22 @@
         <v>0</v>
       </c>
       <c r="C144">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D144">
-        <v>6.413730528533386</v>
+        <v>5.808664500794845</v>
       </c>
       <c r="E144">
-        <v>10.0601723032581</v>
+        <v>11.01945899126518</v>
       </c>
       <c r="F144">
-        <v>12.21138205001378</v>
+        <v>12.41173617355729</v>
       </c>
       <c r="G144">
-        <v>0.003213823146789534</v>
+        <v>0.02299103960716629</v>
       </c>
       <c r="H144">
-        <v>0.1142949506280326</v>
+        <v>0.1111553603745711</v>
       </c>
     </row>
     <row r="145" spans="1:8">
@@ -4196,22 +4196,22 @@
         <v>0</v>
       </c>
       <c r="C145">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D145">
-        <v>6.480785272422295</v>
+        <v>5.867592750624579</v>
       </c>
       <c r="E145">
-        <v>9.596680128689554</v>
+        <v>10.57197838358684</v>
       </c>
       <c r="F145">
-        <v>12.39687796434905</v>
+        <v>12.59658560000239</v>
       </c>
       <c r="G145">
-        <v>0.003142568183102932</v>
+        <v>0.02237617725232876</v>
       </c>
       <c r="H145">
-        <v>0.1137108244105061</v>
+        <v>0.1107155806864986</v>
       </c>
     </row>
     <row r="146" spans="1:8">
@@ -4222,22 +4222,22 @@
         <v>0</v>
       </c>
       <c r="C146">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D146">
-        <v>6.548144231040892</v>
+        <v>5.926848617790089</v>
       </c>
       <c r="E146">
-        <v>9.13076530168718</v>
+        <v>10.1217815019415</v>
       </c>
       <c r="F146">
-        <v>12.58364516334103</v>
+        <v>12.78281365210358</v>
       </c>
       <c r="G146">
-        <v>0.003073033591002877</v>
+        <v>0.02177249573431219</v>
       </c>
       <c r="H146">
-        <v>0.1130819465116651</v>
+        <v>0.1102429543025959</v>
       </c>
     </row>
     <row r="147" spans="1:8">
@@ -4248,22 +4248,22 @@
         <v>0</v>
       </c>
       <c r="C147">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D147">
-        <v>6.615770551983735</v>
+        <v>5.986409032311391</v>
       </c>
       <c r="E147">
-        <v>8.662604018472411</v>
+        <v>9.668991793629591</v>
       </c>
       <c r="F147">
-        <v>12.77160514142212</v>
+        <v>12.97036569510729</v>
       </c>
       <c r="G147">
-        <v>0.003005304868449078</v>
+        <v>0.02118030729318758</v>
       </c>
       <c r="H147">
-        <v>0.1124014533567466</v>
+        <v>0.109733070880611</v>
       </c>
     </row>
     <row r="148" spans="1:8">
@@ -4274,22 +4274,22 @@
         <v>0</v>
       </c>
       <c r="C148">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D148">
-        <v>6.683620935180967</v>
+        <v>6.046247122752642</v>
       </c>
       <c r="E148">
-        <v>8.192404553638516</v>
+        <v>9.213754203815409</v>
       </c>
       <c r="F148">
-        <v>12.96066485048327</v>
+        <v>13.15917735509561</v>
       </c>
       <c r="G148">
-        <v>0.002939489191301957</v>
+        <v>0.02059999932690416</v>
       </c>
       <c r="H148">
-        <v>0.1116611008812805</v>
+        <v>0.1091807309830572</v>
       </c>
     </row>
     <row r="149" spans="1:8">
@@ -4300,22 +4300,22 @@
         <v>0</v>
       </c>
       <c r="C149">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D149">
-        <v>6.751644320944536</v>
+        <v>6.10633152626315</v>
       </c>
       <c r="E149">
-        <v>7.720413773203817</v>
+        <v>8.756239071541632</v>
       </c>
       <c r="F149">
-        <v>13.15071374996145</v>
+        <v>13.34917275514619</v>
       </c>
       <c r="G149">
-        <v>0.002875721426621017</v>
+        <v>0.0200320519151866</v>
       </c>
       <c r="H149">
-        <v>0.1108509082805822</v>
+        <v>0.1085797654558652</v>
       </c>
     </row>
     <row r="150" spans="1:8">
@@ -4326,22 +4326,22 @@
         <v>0</v>
       </c>
       <c r="C150">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D150">
-        <v>6.819780233526887</v>
+        <v>6.166625543866487</v>
       </c>
       <c r="E150">
-        <v>7.246925352032279</v>
+        <v>8.296646897565092</v>
       </c>
       <c r="F150">
-        <v>13.34162008609653</v>
+        <v>13.54026235715356</v>
       </c>
       <c r="G150">
-        <v>0.002814172310230311</v>
+        <v>0.01947706063584732</v>
       </c>
       <c r="H150">
-        <v>0.109958689177836</v>
+        <v>0.1079228042057132</v>
       </c>
     </row>
     <row r="151" spans="1:8">
@@ -4352,22 +4352,22 @@
         <v>0</v>
       </c>
       <c r="C151">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D151">
-        <v>6.887956673919726</v>
+        <v>6.227086085167179</v>
       </c>
       <c r="E151">
-        <v>6.772290221054372</v>
+        <v>7.835214295763728</v>
       </c>
       <c r="F151">
-        <v>13.53322616279254</v>
+        <v>13.73234026881644</v>
       </c>
       <c r="G151">
-        <v>0.002755059747110291</v>
+        <v>0.01893576676640612</v>
       </c>
       <c r="H151">
-        <v>0.1089694279380401</v>
+        <v>0.1072009776547356</v>
       </c>
     </row>
     <row r="152" spans="1:8">
@@ -4378,22 +4378,22 @@
         <v>0</v>
       </c>
       <c r="C152">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D152">
-        <v>6.956087432711479</v>
+        <v>6.287662355832977</v>
       </c>
       <c r="E152">
-        <v>6.29692988252044</v>
+        <v>7.372221392303513</v>
       </c>
       <c r="F152">
-        <v>13.72534231560997</v>
+        <v>13.92528089603631</v>
       </c>
       <c r="G152">
-        <v>0.00269866468355866</v>
+        <v>0.01840909762222236</v>
       </c>
       <c r="H152">
-        <v>0.107864440273888</v>
+        <v>0.1064035275030645</v>
       </c>
     </row>
     <row r="153" spans="1:8">
@@ -4404,22 +4404,22 @@
         <v>0</v>
       </c>
       <c r="C153">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D153">
-        <v>7.024068523598076</v>
+        <v>6.348294199337394</v>
       </c>
       <c r="E153">
-        <v>5.821354068534327</v>
+        <v>6.908001167970691</v>
       </c>
       <c r="F153">
-        <v>13.91773892286118</v>
+        <v>14.1189347172564</v>
       </c>
       <c r="G153">
-        <v>0.002645353938131246</v>
+        <v>0.01789822137366007</v>
       </c>
       <c r="H153">
-        <v>0.1066202314284949</v>
+        <v>0.1055172943135048</v>
       </c>
     </row>
     <row r="154" spans="1:8">
@@ -4430,22 +4430,22 @@
         <v>0</v>
       </c>
       <c r="C154">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D154">
-        <v>7.091773566525355</v>
+        <v>6.408909993346465</v>
       </c>
       <c r="E154">
-        <v>5.346183591167699</v>
+        <v>6.442951303207523</v>
       </c>
       <c r="F154">
-        <v>14.1101360697574</v>
+        <v>14.31312292697898</v>
       </c>
       <c r="G154">
-        <v>0.002595613674114375</v>
+        <v>0.01740462267253083</v>
       </c>
       <c r="H154">
-        <v>0.10520692229706</v>
+        <v>0.1045260358372356</v>
       </c>
     </row>
     <row r="155" spans="1:8">
@@ -4456,22 +4456,22 @@
         <v>0</v>
       </c>
       <c r="C155">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D155">
-        <v>7.159047615692361</v>
+        <v>6.469423929506268</v>
       </c>
       <c r="E155">
-        <v>4.87218087018162</v>
+        <v>5.977549485390234</v>
       </c>
       <c r="F155">
-        <v>14.3021897434827</v>
+        <v>14.50763051543563</v>
       </c>
       <c r="G155">
-        <v>0.002550099753909913</v>
+        <v>0.01693020911109132</v>
       </c>
       <c r="H155">
-        <v>0.1035860548510026</v>
+        <v>0.1034095107602912</v>
       </c>
     </row>
     <row r="156" spans="1:8">
@@ -4482,22 +4482,22 @@
         <v>0</v>
       </c>
       <c r="C156">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D156">
-        <v>7.225698906782377</v>
+        <v>6.529732461370115</v>
       </c>
       <c r="E156">
-        <v>4.400290730516203</v>
+        <v>5.512373386272214</v>
       </c>
       <c r="F156">
-        <v>14.49347338855195</v>
+        <v>14.70219723900211</v>
       </c>
       <c r="G156">
-        <v>0.002509715816171259</v>
+        <v>0.01647746402424996</v>
       </c>
       <c r="H156">
-        <v>0.1017074949334318</v>
+        <v>0.1021422338677312</v>
       </c>
     </row>
     <row r="157" spans="1:8">
@@ -4508,22 +4508,22 @@
         <v>0</v>
       </c>
       <c r="C157">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D157">
-        <v>7.291487347046812</v>
+        <v>6.589709659546396</v>
       </c>
       <c r="E157">
-        <v>3.931697269149757</v>
+        <v>5.048126772852811</v>
       </c>
       <c r="F157">
-        <v>14.68345220359585</v>
+        <v>14.89650582087425</v>
       </c>
       <c r="G157">
-        <v>0.002475737610177295</v>
+        <v>0.01604967066947882</v>
       </c>
       <c r="H157">
-        <v>0.09950502200959205</v>
+        <v>0.1006917660159841</v>
       </c>
     </row>
     <row r="158" spans="1:8">
@@ -4534,22 +4534,22 @@
         <v>0</v>
       </c>
       <c r="C158">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D158">
-        <v>7.356108923995813</v>
+        <v>6.649201039434113</v>
       </c>
       <c r="E158">
-        <v>3.467900854047849</v>
+        <v>4.585674186293045</v>
       </c>
       <c r="F158">
-        <v>14.87144834543594</v>
+        <v>15.09016628362432</v>
       </c>
       <c r="G158">
-        <v>0.002450021239206266</v>
+        <v>0.01565124930646292</v>
       </c>
       <c r="H158">
-        <v>0.09688999763041174</v>
+        <v>0.09901634141045619</v>
       </c>
     </row>
     <row r="159" spans="1:8">
@@ -4560,22 +4560,22 @@
         <v>0</v>
       </c>
       <c r="C159">
-        <v>0.301652706463842</v>
+        <v>0.300613200020739</v>
       </c>
       <c r="D159">
-        <v>7.419173677201023</v>
+        <v>6.70801525057997</v>
       </c>
       <c r="E159">
-        <v>3.01082686239302</v>
+        <v>4.126087612163091</v>
       </c>
       <c r="F159">
-        <v>15.05659180058131</v>
+        <v>15.28269486922189</v>
       </c>
       <c r="G159">
-        <v>0.002435361765760943</v>
+        <v>0.01528828004602542</v>
       </c>
       <c r="H159">
-        <v>0.09374227773308839</v>
+        <v>0.09706154718162337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>